<commit_message>
compiler: Fix the fourth parameter of HLOOKUP and VLOOKUP (Fixes issue 24).
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14460" windowHeight="13080"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>Actual</t>
   </si>
@@ -110,6 +110,42 @@
   </si>
   <si>
     <t>INDEX (1-dim, 2-idx)</t>
+  </si>
+  <si>
+    <t>three</t>
+  </si>
+  <si>
+    <t>один</t>
+  </si>
+  <si>
+    <t>два</t>
+  </si>
+  <si>
+    <t>три</t>
+  </si>
+  <si>
+    <t>eins</t>
+  </si>
+  <si>
+    <t>zwei</t>
+  </si>
+  <si>
+    <t>drei</t>
+  </si>
+  <si>
+    <t>VLOOKUP (equality)</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>четыре</t>
+  </si>
+  <si>
+    <t>vier</t>
+  </si>
+  <si>
+    <t>HLOOKUP (equality)</t>
   </si>
 </sst>
 </file>
@@ -487,7 +523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q179"/>
+  <dimension ref="A1:Q187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +531,12 @@
   <cols>
     <col min="1" max="1" width="15.625" customWidth="1"/>
     <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="5.375" customWidth="1"/>
+    <col min="3" max="3" width="5.875" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="7" customWidth="1"/>
+    <col min="6" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="9.25" customWidth="1"/>
+    <col min="8" max="9" width="5.375" customWidth="1"/>
     <col min="10" max="10" width="10.25" style="1" customWidth="1"/>
     <col min="11" max="11" width="24.25" customWidth="1"/>
   </cols>
@@ -3474,62 +3515,68 @@
       </c>
     </row>
     <row r="114" spans="1:17">
-      <c r="A114">
-        <v>22</v>
-      </c>
-      <c r="B114">
-        <f>VLOOKUP(C114,D$114:F$116,3)</f>
-        <v>22</v>
-      </c>
-      <c r="C114">
-        <v>29</v>
-      </c>
-      <c r="D114">
-        <v>10</v>
-      </c>
-      <c r="E114">
-        <v>11</v>
-      </c>
-      <c r="F114">
-        <v>21</v>
+      <c r="A114" t="s">
+        <v>12</v>
+      </c>
+      <c r="B114" t="str">
+        <f>HLOOKUP(C114,D$114:G$116,1,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C114" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" t="s">
+        <v>13</v>
+      </c>
+      <c r="F114" t="s">
+        <v>32</v>
+      </c>
+      <c r="G114" t="s">
+        <v>40</v>
       </c>
       <c r="J114" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K114" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="L114" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P114" t="b">
-        <f t="shared" ref="P114:P121" si="11">OR(ISBLANK(B114),IF(ISERROR(B114),ERROR.TYPE(B114)=IF(ISBLANK(M114),ERROR.TYPE(A114),ERROR.TYPE(M114)),IF(ISBLANK(M114),AND(NOT(ISBLANK(A114)),A114=B114),B114=M114)))</f>
+        <f t="shared" ref="P114:P116" si="11">OR(ISBLANK(B114),IF(ISERROR(B114),ERROR.TYPE(B114)=IF(ISBLANK(M114),ERROR.TYPE(A114),ERROR.TYPE(M114)),IF(ISBLANK(M114),AND(NOT(ISBLANK(A114)),A114=B114),B114=M114)))</f>
         <v>1</v>
       </c>
       <c r="Q114" t="b">
-        <f t="shared" ref="Q114:Q121" si="12">IF(ISBLANK(O114),IF(ISERROR(P114),FALSE,P114),O114)</f>
+        <f t="shared" ref="Q114:Q116" si="12">IF(ISBLANK(O114),IF(ISERROR(P114),FALSE,P114),O114)</f>
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:17">
-      <c r="A115">
-        <v>23</v>
-      </c>
-      <c r="B115">
-        <f>VLOOKUP(C115,D$114:F$116,3)</f>
-        <v>23</v>
-      </c>
-      <c r="C115">
-        <v>30</v>
-      </c>
-      <c r="D115">
-        <v>20</v>
-      </c>
-      <c r="E115">
-        <v>12</v>
-      </c>
-      <c r="F115">
-        <v>22</v>
+      <c r="A115" t="s">
+        <v>35</v>
+      </c>
+      <c r="B115" t="str">
+        <f>HLOOKUP(C115,D$114:G$116,2,FALSE)</f>
+        <v>три</v>
+      </c>
+      <c r="C115" t="s">
+        <v>32</v>
+      </c>
+      <c r="D115" t="s">
+        <v>33</v>
+      </c>
+      <c r="E115" t="s">
+        <v>34</v>
+      </c>
+      <c r="F115" t="s">
+        <v>35</v>
+      </c>
+      <c r="G115" t="s">
+        <v>41</v>
       </c>
       <c r="J115" s="1">
         <v>1</v>
@@ -3544,24 +3591,27 @@
       </c>
     </row>
     <row r="116" spans="1:17">
-      <c r="A116">
-        <v>23</v>
-      </c>
-      <c r="B116">
-        <f>VLOOKUP(C116,D$114:F$116,3)</f>
-        <v>23</v>
-      </c>
-      <c r="C116">
-        <v>31</v>
-      </c>
-      <c r="D116">
-        <v>30</v>
-      </c>
-      <c r="E116">
-        <v>13</v>
-      </c>
-      <c r="F116">
-        <v>23</v>
+      <c r="A116" t="s">
+        <v>42</v>
+      </c>
+      <c r="B116" t="str">
+        <f>HLOOKUP(C116,D$114:G$116,3,FALSE)</f>
+        <v>vier</v>
+      </c>
+      <c r="C116" t="s">
+        <v>40</v>
+      </c>
+      <c r="D116" t="s">
+        <v>36</v>
+      </c>
+      <c r="E116" t="s">
+        <v>37</v>
+      </c>
+      <c r="F116" t="s">
+        <v>38</v>
+      </c>
+      <c r="G116" t="s">
+        <v>42</v>
       </c>
       <c r="J116" s="1">
         <v>1</v>
@@ -3575,55 +3625,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
-      <c r="A117">
-        <v>20</v>
-      </c>
-      <c r="B117">
-        <f>VLOOKUP(C117,D$114:F$116,D117)</f>
-        <v>20</v>
-      </c>
-      <c r="C117">
-        <v>29</v>
-      </c>
-      <c r="D117">
-        <v>1</v>
-      </c>
-      <c r="J117" s="1">
-        <v>2</v>
-      </c>
-      <c r="P117" t="b">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Q117" t="b">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
     <row r="118" spans="1:17">
       <c r="A118">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B118">
-        <f>VLOOKUP(C118,D$114:F$116,D118)</f>
-        <v>13</v>
+        <f>VLOOKUP(C118,D$118:F$120,3)</f>
+        <v>22</v>
       </c>
       <c r="C118">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D118">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="E118">
+        <v>11</v>
+      </c>
+      <c r="F118">
+        <v>21</v>
       </c>
       <c r="J118" s="1">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="K118" t="s">
+        <v>25</v>
+      </c>
+      <c r="L118" t="s">
+        <v>25</v>
       </c>
       <c r="P118" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="P118:P125" si="13">OR(ISBLANK(B118),IF(ISERROR(B118),ERROR.TYPE(B118)=IF(ISBLANK(M118),ERROR.TYPE(A118),ERROR.TYPE(M118)),IF(ISBLANK(M118),AND(NOT(ISBLANK(A118)),A118=B118),B118=M118)))</f>
         <v>1</v>
       </c>
       <c r="Q118" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="Q118:Q125" si="14">IF(ISBLANK(O118),IF(ISERROR(P118),FALSE,P118),O118)</f>
         <v>1</v>
       </c>
     </row>
@@ -3632,338 +3668,535 @@
         <v>23</v>
       </c>
       <c r="B119">
-        <f>VLOOKUP(C119,D$114:F$116,D119)</f>
+        <f>VLOOKUP(C119,D$118:F$120,3)</f>
         <v>23</v>
       </c>
       <c r="C119">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D119">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="E119">
+        <v>12</v>
+      </c>
+      <c r="F119">
+        <v>22</v>
       </c>
       <c r="J119" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P119" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="Q119" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:17">
-      <c r="A120" t="s">
-        <v>28</v>
-      </c>
-      <c r="B120" t="e">
-        <f>VLOOKUP(C120,D$114:F$116,D120)</f>
-        <v>#VALUE!</v>
+      <c r="A120">
+        <v>23</v>
+      </c>
+      <c r="B120">
+        <f>VLOOKUP(C120,D$118:F$120,3)</f>
+        <v>23</v>
       </c>
       <c r="C120">
         <v>31</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="E120">
+        <v>13</v>
+      </c>
+      <c r="F120">
+        <v>23</v>
       </c>
       <c r="J120" s="1">
-        <v>2</v>
-      </c>
-      <c r="M120" s="3" t="e">
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="P120" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="Q120" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:17">
-      <c r="A121" t="s">
-        <v>28</v>
-      </c>
-      <c r="B121" t="e">
-        <f>VLOOKUP(C121,D$114:F$116,D121)</f>
-        <v>#REF!</v>
+      <c r="A121">
+        <v>20</v>
+      </c>
+      <c r="B121">
+        <f>VLOOKUP(C121,D$118:F$120,D121)</f>
+        <v>20</v>
       </c>
       <c r="C121">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D121">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J121" s="1">
         <v>2</v>
       </c>
-      <c r="M121" s="3" t="e">
-        <v>#REF!</v>
-      </c>
       <c r="P121" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="Q121" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:17">
-      <c r="M122" s="3"/>
+      <c r="A122">
+        <v>13</v>
+      </c>
+      <c r="B122">
+        <f>VLOOKUP(C122,D$118:F$120,D122)</f>
+        <v>13</v>
+      </c>
+      <c r="C122">
+        <v>30</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+      <c r="J122" s="1">
+        <v>2</v>
+      </c>
+      <c r="P122" t="b">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="Q122" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:17">
       <c r="A123">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B123">
-        <f t="shared" ref="B123:B128" si="13">CHOOSE(C123,D123,E123,F123)</f>
-        <v>11</v>
+        <f>VLOOKUP(C123,D$118:F$120,D123)</f>
+        <v>23</v>
       </c>
       <c r="C123">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="D123">
-        <v>11</v>
-      </c>
-      <c r="E123">
-        <v>12</v>
-      </c>
-      <c r="F123">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="J123" s="1">
-        <v>4</v>
-      </c>
-      <c r="K123" t="s">
-        <v>26</v>
-      </c>
-      <c r="L123" t="s">
-        <v>26</v>
-      </c>
-      <c r="M123" s="3"/>
+        <v>2</v>
+      </c>
       <c r="P123" t="b">
-        <f t="shared" ref="P123:P128" si="14">OR(ISBLANK(B123),IF(ISERROR(B123),ERROR.TYPE(B123)=IF(ISBLANK(M123),ERROR.TYPE(A123),ERROR.TYPE(M123)),IF(ISBLANK(M123),AND(NOT(ISBLANK(A123)),A123=B123),B123=M123)))</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="Q123" t="b">
-        <f t="shared" ref="Q123:Q128" si="15">IF(ISBLANK(O123),IF(ISERROR(P123),FALSE,P123),O123)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:17">
-      <c r="A124">
-        <v>22</v>
-      </c>
-      <c r="B124">
+      <c r="A124" t="s">
+        <v>28</v>
+      </c>
+      <c r="B124" t="e">
+        <f>VLOOKUP(C124,D$118:F$120,D124)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C124">
+        <v>31</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1">
+        <v>2</v>
+      </c>
+      <c r="M124" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P124" t="b">
         <f t="shared" si="13"/>
-        <v>22</v>
-      </c>
-      <c r="C124">
-        <v>2</v>
-      </c>
-      <c r="D124">
-        <v>21</v>
-      </c>
-      <c r="E124">
-        <v>22</v>
-      </c>
-      <c r="F124">
-        <v>23</v>
-      </c>
-      <c r="J124" s="1">
-        <v>4</v>
-      </c>
-      <c r="P124" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q124" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="Q124" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="125" spans="1:17">
-      <c r="A125">
-        <v>33</v>
-      </c>
-      <c r="B125">
+      <c r="A125" t="s">
+        <v>28</v>
+      </c>
+      <c r="B125" t="e">
+        <f>VLOOKUP(C125,D$118:F$120,D125)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C125">
+        <v>31</v>
+      </c>
+      <c r="D125">
+        <v>4</v>
+      </c>
+      <c r="J125" s="1">
+        <v>2</v>
+      </c>
+      <c r="M125" s="3" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="P125" t="b">
         <f t="shared" si="13"/>
-        <v>33</v>
-      </c>
-      <c r="C125">
-        <v>3</v>
-      </c>
-      <c r="D125">
-        <v>31</v>
-      </c>
-      <c r="E125">
-        <v>32</v>
-      </c>
-      <c r="F125">
-        <v>33</v>
-      </c>
-      <c r="J125" s="1">
-        <v>4</v>
-      </c>
-      <c r="P125" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q125" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="Q125" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="126" spans="1:17">
-      <c r="A126" t="s">
-        <v>28</v>
-      </c>
-      <c r="B126" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C126">
-        <v>4</v>
-      </c>
-      <c r="D126">
-        <v>11</v>
-      </c>
-      <c r="E126">
-        <v>12</v>
-      </c>
-      <c r="F126">
-        <v>13</v>
-      </c>
-      <c r="J126" s="1">
-        <v>4</v>
-      </c>
-      <c r="M126" s="3" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P126" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Q126" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
+      <c r="M126" s="3"/>
     </row>
     <row r="127" spans="1:17">
       <c r="A127" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" t="str">
+        <f>VLOOKUP(C127,D$127:F$129,1,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C127" t="s">
+        <v>12</v>
+      </c>
+      <c r="D127" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" t="s">
+        <v>33</v>
+      </c>
+      <c r="F127" t="s">
+        <v>36</v>
+      </c>
+      <c r="J127" s="1">
+        <v>4</v>
+      </c>
+      <c r="K127" t="s">
+        <v>39</v>
+      </c>
+      <c r="L127" t="s">
+        <v>25</v>
+      </c>
+      <c r="P127" t="b">
+        <f t="shared" ref="P127:P129" si="15">OR(ISBLANK(B127),IF(ISERROR(B127),ERROR.TYPE(B127)=IF(ISBLANK(M127),ERROR.TYPE(A127),ERROR.TYPE(M127)),IF(ISBLANK(M127),AND(NOT(ISBLANK(A127)),A127=B127),B127=M127)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q127" t="b">
+        <f t="shared" ref="Q127:Q129" si="16">IF(ISBLANK(O127),IF(ISERROR(P127),FALSE,P127),O127)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17">
+      <c r="A128" t="s">
+        <v>34</v>
+      </c>
+      <c r="B128" t="str">
+        <f>VLOOKUP(C128,D$127:F$129,2,FALSE)</f>
+        <v>два</v>
+      </c>
+      <c r="C128" t="s">
+        <v>13</v>
+      </c>
+      <c r="D128" t="s">
+        <v>13</v>
+      </c>
+      <c r="E128" t="s">
+        <v>34</v>
+      </c>
+      <c r="F128" t="s">
+        <v>37</v>
+      </c>
+      <c r="J128" s="1">
+        <v>1</v>
+      </c>
+      <c r="P128" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q128" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
+      <c r="A129" t="s">
+        <v>38</v>
+      </c>
+      <c r="B129" t="str">
+        <f>VLOOKUP(C129,D$127:F$129,3,FALSE)</f>
+        <v>drei</v>
+      </c>
+      <c r="C129" t="s">
+        <v>32</v>
+      </c>
+      <c r="D129" t="s">
+        <v>32</v>
+      </c>
+      <c r="E129" t="s">
+        <v>35</v>
+      </c>
+      <c r="F129" t="s">
+        <v>38</v>
+      </c>
+      <c r="J129" s="1">
+        <v>1</v>
+      </c>
+      <c r="P129" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="Q129" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17">
+      <c r="M130" s="3"/>
+    </row>
+    <row r="131" spans="1:17">
+      <c r="A131">
+        <v>11</v>
+      </c>
+      <c r="B131">
+        <f t="shared" ref="B131:B136" si="17">CHOOSE(C131,D131,E131,F131)</f>
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>11</v>
+      </c>
+      <c r="E131">
+        <v>12</v>
+      </c>
+      <c r="F131">
+        <v>13</v>
+      </c>
+      <c r="J131" s="1">
+        <v>4</v>
+      </c>
+      <c r="K131" t="s">
+        <v>26</v>
+      </c>
+      <c r="L131" t="s">
+        <v>26</v>
+      </c>
+      <c r="M131" s="3"/>
+      <c r="P131" t="b">
+        <f t="shared" ref="P131:P136" si="18">OR(ISBLANK(B131),IF(ISERROR(B131),ERROR.TYPE(B131)=IF(ISBLANK(M131),ERROR.TYPE(A131),ERROR.TYPE(M131)),IF(ISBLANK(M131),AND(NOT(ISBLANK(A131)),A131=B131),B131=M131)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q131" t="b">
+        <f t="shared" ref="Q131:Q136" si="19">IF(ISBLANK(O131),IF(ISERROR(P131),FALSE,P131),O131)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
+      <c r="A132">
+        <v>22</v>
+      </c>
+      <c r="B132">
+        <f t="shared" si="17"/>
+        <v>22</v>
+      </c>
+      <c r="C132">
+        <v>2</v>
+      </c>
+      <c r="D132">
+        <v>21</v>
+      </c>
+      <c r="E132">
+        <v>22</v>
+      </c>
+      <c r="F132">
+        <v>23</v>
+      </c>
+      <c r="J132" s="1">
+        <v>4</v>
+      </c>
+      <c r="P132" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q132" t="b">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:17">
+      <c r="A133">
+        <v>33</v>
+      </c>
+      <c r="B133">
+        <f t="shared" si="17"/>
+        <v>33</v>
+      </c>
+      <c r="C133">
+        <v>3</v>
+      </c>
+      <c r="D133">
+        <v>31</v>
+      </c>
+      <c r="E133">
+        <v>32</v>
+      </c>
+      <c r="F133">
+        <v>33</v>
+      </c>
+      <c r="J133" s="1">
+        <v>4</v>
+      </c>
+      <c r="P133" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q133" t="b">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:17">
+      <c r="A134" t="s">
         <v>28</v>
       </c>
-      <c r="B127" t="e">
-        <f t="shared" si="13"/>
+      <c r="B134" t="e">
+        <f t="shared" si="17"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C127">
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134">
+        <v>11</v>
+      </c>
+      <c r="E134">
+        <v>12</v>
+      </c>
+      <c r="F134">
+        <v>13</v>
+      </c>
+      <c r="J134" s="1">
+        <v>4</v>
+      </c>
+      <c r="M134" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P134" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q134" t="b">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:17">
+      <c r="A135" t="s">
+        <v>28</v>
+      </c>
+      <c r="B135" t="e">
+        <f t="shared" si="17"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C135">
         <v>0</v>
       </c>
-      <c r="D127">
-        <v>11</v>
-      </c>
-      <c r="E127">
-        <v>12</v>
-      </c>
-      <c r="F127">
+      <c r="D135">
+        <v>11</v>
+      </c>
+      <c r="E135">
+        <v>12</v>
+      </c>
+      <c r="F135">
         <v>13</v>
       </c>
-      <c r="J127" s="1">
-        <v>4</v>
-      </c>
-      <c r="M127" s="3" t="e">
+      <c r="J135" s="1">
+        <v>4</v>
+      </c>
+      <c r="M135" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P127" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Q127" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17">
-      <c r="A128">
-        <v>12</v>
-      </c>
-      <c r="B128">
-        <f t="shared" si="13"/>
-        <v>12</v>
-      </c>
-      <c r="C128">
+      <c r="P135" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q135" t="b">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17">
+      <c r="A136">
+        <v>12</v>
+      </c>
+      <c r="B136">
+        <f t="shared" si="17"/>
+        <v>12</v>
+      </c>
+      <c r="C136">
         <v>2.99</v>
       </c>
-      <c r="D128">
-        <v>11</v>
-      </c>
-      <c r="E128">
-        <v>12</v>
-      </c>
-      <c r="F128">
+      <c r="D136">
+        <v>11</v>
+      </c>
+      <c r="E136">
+        <v>12</v>
+      </c>
+      <c r="F136">
         <v>13</v>
       </c>
-      <c r="J128" s="1">
-        <v>4</v>
-      </c>
-      <c r="P128" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Q128" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="13:13">
-      <c r="M142" s="3"/>
-    </row>
-    <row r="146" spans="13:13">
-      <c r="M146" s="3"/>
-    </row>
-    <row r="148" spans="13:13">
-      <c r="M148" s="3"/>
-    </row>
-    <row r="149" spans="13:13">
-      <c r="M149" s="3"/>
-    </row>
-    <row r="151" spans="13:13">
-      <c r="M151" s="3"/>
-    </row>
-    <row r="153" spans="13:13">
-      <c r="M153" s="3"/>
+      <c r="J136" s="1">
+        <v>4</v>
+      </c>
+      <c r="P136" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="Q136" t="b">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="13:13">
+      <c r="M150" s="3"/>
     </row>
     <row r="154" spans="13:13">
       <c r="M154" s="3"/>
     </row>
-    <row r="158" spans="13:13">
-      <c r="M158" s="3"/>
+    <row r="156" spans="13:13">
+      <c r="M156" s="3"/>
+    </row>
+    <row r="157" spans="13:13">
+      <c r="M157" s="3"/>
     </row>
     <row r="159" spans="13:13">
       <c r="M159" s="3"/>
     </row>
-    <row r="160" spans="13:13">
-      <c r="M160" s="3"/>
-    </row>
     <row r="161" spans="13:13">
       <c r="M161" s="3"/>
     </row>
     <row r="162" spans="13:13">
       <c r="M162" s="3"/>
     </row>
-    <row r="163" spans="13:13">
-      <c r="M163" s="3"/>
-    </row>
-    <row r="164" spans="13:13">
-      <c r="M164" s="3"/>
-    </row>
-    <row r="165" spans="13:13">
-      <c r="M165" s="3"/>
-    </row>
     <row r="166" spans="13:13">
       <c r="M166" s="3"/>
     </row>
@@ -4006,9 +4239,33 @@
     <row r="179" spans="13:13">
       <c r="M179" s="3"/>
     </row>
+    <row r="180" spans="13:13">
+      <c r="M180" s="3"/>
+    </row>
+    <row r="181" spans="13:13">
+      <c r="M181" s="3"/>
+    </row>
+    <row r="182" spans="13:13">
+      <c r="M182" s="3"/>
+    </row>
+    <row r="183" spans="13:13">
+      <c r="M183" s="3"/>
+    </row>
+    <row r="184" spans="13:13">
+      <c r="M184" s="3"/>
+    </row>
+    <row r="185" spans="13:13">
+      <c r="M185" s="3"/>
+    </row>
+    <row r="186" spans="13:13">
+      <c r="M186" s="3"/>
+    </row>
+    <row r="187" spans="13:13">
+      <c r="M187" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A10009">
+  <conditionalFormatting sqref="A2:A10017">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
@@ -4016,12 +4273,12 @@
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I10009">
+  <conditionalFormatting sqref="C2:I10017">
     <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M10009">
+  <conditionalFormatting sqref="M2:M10017">
     <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
     </cfRule>

</xml_diff>

<commit_message>
test: Add reference tests for strict text equality for HLOOKUP and VLOOKUP (tests for issue 25).
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
   <si>
     <t>Actual</t>
   </si>
@@ -145,7 +145,16 @@
     <t>vier</t>
   </si>
   <si>
+    <t>five</t>
+  </si>
+  <si>
     <t>HLOOKUP (equality)</t>
+  </si>
+  <si>
+    <t>!STR:FE</t>
+  </si>
+  <si>
+    <t>!STR:NA</t>
   </si>
 </sst>
 </file>
@@ -204,7 +213,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -523,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q187"/>
+  <dimension ref="A1:Q199"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3541,17 +3564,17 @@
         <v>5</v>
       </c>
       <c r="K114" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L114" t="s">
         <v>24</v>
       </c>
       <c r="P114" t="b">
-        <f t="shared" ref="P114:P116" si="11">OR(ISBLANK(B114),IF(ISERROR(B114),ERROR.TYPE(B114)=IF(ISBLANK(M114),ERROR.TYPE(A114),ERROR.TYPE(M114)),IF(ISBLANK(M114),AND(NOT(ISBLANK(A114)),A114=B114),B114=M114)))</f>
+        <f t="shared" ref="P114:P121" si="11">OR(ISBLANK(B114),IF(ISERROR(B114),ERROR.TYPE(B114)=IF(ISBLANK(M114),ERROR.TYPE(A114),ERROR.TYPE(M114)),IF(ISBLANK(M114),AND(NOT(ISBLANK(A114)),A114=B114),B114=M114)))</f>
         <v>1</v>
       </c>
       <c r="Q114" t="b">
-        <f t="shared" ref="Q114:Q116" si="12">IF(ISBLANK(O114),IF(ISERROR(P114),FALSE,P114),O114)</f>
+        <f t="shared" ref="Q114:Q122" si="12">IF(ISBLANK(O114),IF(ISERROR(P114),FALSE,P114),O114)</f>
         <v>1</v>
       </c>
     </row>
@@ -3625,574 +3648,886 @@
         <v>1</v>
       </c>
     </row>
+    <row r="117" spans="1:17">
+      <c r="A117" t="s">
+        <v>12</v>
+      </c>
+      <c r="B117" t="str">
+        <f t="shared" ref="B117:B122" si="13">HLOOKUP(C117,D$114:G$116,D117,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C117" t="s">
+        <v>12</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+      <c r="J117" s="1">
+        <v>2</v>
+      </c>
+      <c r="P117" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q117" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
     <row r="118" spans="1:17">
-      <c r="A118">
+      <c r="A118" t="s">
+        <v>35</v>
+      </c>
+      <c r="B118" t="str">
+        <f t="shared" si="13"/>
+        <v>три</v>
+      </c>
+      <c r="C118" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118">
+        <v>2</v>
+      </c>
+      <c r="J118" s="1">
+        <v>2</v>
+      </c>
+      <c r="P118" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q118" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
+      <c r="A119" t="s">
+        <v>42</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" si="13"/>
+        <v>vier</v>
+      </c>
+      <c r="C119" t="s">
+        <v>40</v>
+      </c>
+      <c r="D119">
+        <v>3</v>
+      </c>
+      <c r="J119" s="1">
+        <v>2</v>
+      </c>
+      <c r="P119" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q119" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
+      <c r="A120" t="s">
+        <v>46</v>
+      </c>
+      <c r="B120" t="e">
+        <f t="shared" si="13"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C120" t="s">
+        <v>43</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+      <c r="J120" s="1">
+        <v>2</v>
+      </c>
+      <c r="M120" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P120" t="b">
+        <f>OR(ISBLANK(B120),IF(ISERROR(B120),ERROR.TYPE(B120)=IF(ISBLANK(M120),ERROR.TYPE(A120),ERROR.TYPE(M120)),IF(ISBLANK(M120),AND(NOT(ISBLANK(A120)),A120=B120),B120=M120)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q120" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17">
+      <c r="A121" t="s">
+        <v>45</v>
+      </c>
+      <c r="B121" t="e">
+        <f t="shared" si="13"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C121" t="s">
+        <v>12</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
+        <v>2</v>
+      </c>
+      <c r="M121" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P121" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q121" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17">
+      <c r="A122" t="s">
+        <v>45</v>
+      </c>
+      <c r="B122" t="e">
+        <f t="shared" si="13"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C122" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122">
+        <v>4</v>
+      </c>
+      <c r="J122" s="1">
+        <v>2</v>
+      </c>
+      <c r="M122" s="3" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="P122" t="b">
+        <f>OR(ISBLANK(B122),IF(ISERROR(B122),ERROR.TYPE(B122)=IF(ISBLANK(M122),ERROR.TYPE(A122),ERROR.TYPE(M122)),IF(ISBLANK(M122),AND(NOT(ISBLANK(A122)),A122=B122),B122=M122)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q122" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17">
+      <c r="A124">
         <v>22</v>
       </c>
-      <c r="B118">
-        <f>VLOOKUP(C118,D$118:F$120,3)</f>
+      <c r="B124">
+        <f>VLOOKUP(C124,D$124:F$126,3)</f>
         <v>22</v>
       </c>
-      <c r="C118">
+      <c r="C124">
         <v>29</v>
       </c>
-      <c r="D118">
+      <c r="D124">
         <v>10</v>
       </c>
-      <c r="E118">
+      <c r="E124">
         <v>11</v>
       </c>
-      <c r="F118">
+      <c r="F124">
         <v>21</v>
       </c>
-      <c r="J118" s="1">
-        <v>4</v>
-      </c>
-      <c r="K118" t="s">
+      <c r="J124" s="1">
+        <v>4</v>
+      </c>
+      <c r="K124" t="s">
         <v>25</v>
       </c>
-      <c r="L118" t="s">
+      <c r="L124" t="s">
         <v>25</v>
       </c>
-      <c r="P118" t="b">
-        <f t="shared" ref="P118:P125" si="13">OR(ISBLANK(B118),IF(ISERROR(B118),ERROR.TYPE(B118)=IF(ISBLANK(M118),ERROR.TYPE(A118),ERROR.TYPE(M118)),IF(ISBLANK(M118),AND(NOT(ISBLANK(A118)),A118=B118),B118=M118)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q118" t="b">
-        <f t="shared" ref="Q118:Q125" si="14">IF(ISBLANK(O118),IF(ISERROR(P118),FALSE,P118),O118)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:17">
-      <c r="A119">
+      <c r="P124" t="b">
+        <f t="shared" ref="P124:P131" si="14">OR(ISBLANK(B124),IF(ISERROR(B124),ERROR.TYPE(B124)=IF(ISBLANK(M124),ERROR.TYPE(A124),ERROR.TYPE(M124)),IF(ISBLANK(M124),AND(NOT(ISBLANK(A124)),A124=B124),B124=M124)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q124" t="b">
+        <f t="shared" ref="Q124:Q131" si="15">IF(ISBLANK(O124),IF(ISERROR(P124),FALSE,P124),O124)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="A125">
         <v>23</v>
       </c>
-      <c r="B119">
-        <f>VLOOKUP(C119,D$118:F$120,3)</f>
+      <c r="B125">
+        <f>VLOOKUP(C125,D$124:F$126,3)</f>
         <v>23</v>
       </c>
-      <c r="C119">
+      <c r="C125">
         <v>30</v>
       </c>
-      <c r="D119">
+      <c r="D125">
         <v>20</v>
       </c>
-      <c r="E119">
-        <v>12</v>
-      </c>
-      <c r="F119">
+      <c r="E125">
+        <v>12</v>
+      </c>
+      <c r="F125">
         <v>22</v>
       </c>
-      <c r="J119" s="1">
-        <v>1</v>
-      </c>
-      <c r="P119" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q119" t="b">
+      <c r="J125" s="1">
+        <v>1</v>
+      </c>
+      <c r="P125" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:17">
-      <c r="A120">
+      <c r="Q125" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
+      <c r="A126">
         <v>23</v>
       </c>
-      <c r="B120">
-        <f>VLOOKUP(C120,D$118:F$120,3)</f>
+      <c r="B126">
+        <f>VLOOKUP(C126,D$124:F$126,3)</f>
         <v>23</v>
       </c>
-      <c r="C120">
+      <c r="C126">
         <v>31</v>
       </c>
-      <c r="D120">
+      <c r="D126">
         <v>30</v>
       </c>
-      <c r="E120">
+      <c r="E126">
         <v>13</v>
       </c>
-      <c r="F120">
+      <c r="F126">
         <v>23</v>
       </c>
-      <c r="J120" s="1">
-        <v>1</v>
-      </c>
-      <c r="P120" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q120" t="b">
+      <c r="J126" s="1">
+        <v>1</v>
+      </c>
+      <c r="P126" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:17">
-      <c r="A121">
+      <c r="Q126" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
+      <c r="A127">
         <v>20</v>
       </c>
-      <c r="B121">
-        <f>VLOOKUP(C121,D$118:F$120,D121)</f>
+      <c r="B127">
+        <f>VLOOKUP(C127,D$124:F$126,D127)</f>
         <v>20</v>
       </c>
-      <c r="C121">
+      <c r="C127">
         <v>29</v>
       </c>
-      <c r="D121">
-        <v>1</v>
-      </c>
-      <c r="J121" s="1">
-        <v>2</v>
-      </c>
-      <c r="P121" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q121" t="b">
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="J127" s="1">
+        <v>2</v>
+      </c>
+      <c r="P127" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:17">
-      <c r="A122">
+      <c r="Q127" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:17">
+      <c r="A128">
         <v>13</v>
       </c>
-      <c r="B122">
-        <f>VLOOKUP(C122,D$118:F$120,D122)</f>
+      <c r="B128">
+        <f>VLOOKUP(C128,D$124:F$126,D128)</f>
         <v>13</v>
       </c>
-      <c r="C122">
+      <c r="C128">
         <v>30</v>
       </c>
-      <c r="D122">
-        <v>2</v>
-      </c>
-      <c r="J122" s="1">
-        <v>2</v>
-      </c>
-      <c r="P122" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q122" t="b">
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="J128" s="1">
+        <v>2</v>
+      </c>
+      <c r="P128" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:17">
-      <c r="A123">
+      <c r="Q128" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17">
+      <c r="A129">
         <v>23</v>
       </c>
-      <c r="B123">
-        <f>VLOOKUP(C123,D$118:F$120,D123)</f>
+      <c r="B129">
+        <f>VLOOKUP(C129,D$124:F$126,D129)</f>
         <v>23</v>
       </c>
-      <c r="C123">
+      <c r="C129">
         <v>31</v>
       </c>
-      <c r="D123">
+      <c r="D129">
         <v>3</v>
       </c>
-      <c r="J123" s="1">
-        <v>2</v>
-      </c>
-      <c r="P123" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q123" t="b">
+      <c r="J129" s="1">
+        <v>2</v>
+      </c>
+      <c r="P129" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:17">
-      <c r="A124" t="s">
+      <c r="Q129" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17">
+      <c r="A130" t="s">
         <v>28</v>
       </c>
-      <c r="B124" t="e">
-        <f>VLOOKUP(C124,D$118:F$120,D124)</f>
+      <c r="B130" t="e">
+        <f>VLOOKUP(C130,D$124:F$126,D130)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="C124">
+      <c r="C130">
         <v>31</v>
       </c>
-      <c r="D124">
+      <c r="D130">
         <v>0</v>
       </c>
-      <c r="J124" s="1">
-        <v>2</v>
-      </c>
-      <c r="M124" s="3" t="e">
+      <c r="J130" s="1">
+        <v>2</v>
+      </c>
+      <c r="M130" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P124" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q124" t="b">
+      <c r="P130" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:17">
-      <c r="A125" t="s">
+      <c r="Q130" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17">
+      <c r="A131" t="s">
         <v>28</v>
       </c>
-      <c r="B125" t="e">
-        <f>VLOOKUP(C125,D$118:F$120,D125)</f>
+      <c r="B131" t="e">
+        <f>VLOOKUP(C131,D$124:F$126,D131)</f>
         <v>#REF!</v>
       </c>
-      <c r="C125">
+      <c r="C131">
         <v>31</v>
       </c>
-      <c r="D125">
-        <v>4</v>
-      </c>
-      <c r="J125" s="1">
-        <v>2</v>
-      </c>
-      <c r="M125" s="3" t="e">
+      <c r="D131">
+        <v>4</v>
+      </c>
+      <c r="J131" s="1">
+        <v>2</v>
+      </c>
+      <c r="M131" s="3" t="e">
         <v>#REF!</v>
       </c>
-      <c r="P125" t="b">
-        <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="Q125" t="b">
+      <c r="P131" t="b">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:17">
-      <c r="M126" s="3"/>
-    </row>
-    <row r="127" spans="1:17">
-      <c r="A127" t="s">
-        <v>12</v>
-      </c>
-      <c r="B127" t="str">
-        <f>VLOOKUP(C127,D$127:F$129,1,FALSE)</f>
+      <c r="Q131" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17">
+      <c r="M132" s="3"/>
+    </row>
+    <row r="133" spans="1:17">
+      <c r="A133" t="s">
+        <v>12</v>
+      </c>
+      <c r="B133" t="str">
+        <f>VLOOKUP(C133,D$133:F$135,1,FALSE)</f>
         <v>one</v>
       </c>
-      <c r="C127" t="s">
-        <v>12</v>
-      </c>
-      <c r="D127" t="s">
-        <v>12</v>
-      </c>
-      <c r="E127" t="s">
+      <c r="C133" t="s">
+        <v>12</v>
+      </c>
+      <c r="D133" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" t="s">
         <v>33</v>
       </c>
-      <c r="F127" t="s">
+      <c r="F133" t="s">
         <v>36</v>
       </c>
-      <c r="J127" s="1">
-        <v>4</v>
-      </c>
-      <c r="K127" t="s">
+      <c r="J133" s="1">
+        <v>4</v>
+      </c>
+      <c r="K133" t="s">
         <v>39</v>
       </c>
-      <c r="L127" t="s">
+      <c r="L133" t="s">
         <v>25</v>
       </c>
-      <c r="P127" t="b">
-        <f t="shared" ref="P127:P129" si="15">OR(ISBLANK(B127),IF(ISERROR(B127),ERROR.TYPE(B127)=IF(ISBLANK(M127),ERROR.TYPE(A127),ERROR.TYPE(M127)),IF(ISBLANK(M127),AND(NOT(ISBLANK(A127)),A127=B127),B127=M127)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q127" t="b">
-        <f t="shared" ref="Q127:Q129" si="16">IF(ISBLANK(O127),IF(ISERROR(P127),FALSE,P127),O127)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:17">
-      <c r="A128" t="s">
-        <v>34</v>
-      </c>
-      <c r="B128" t="str">
-        <f>VLOOKUP(C128,D$127:F$129,2,FALSE)</f>
-        <v>два</v>
-      </c>
-      <c r="C128" t="s">
-        <v>13</v>
-      </c>
-      <c r="D128" t="s">
-        <v>13</v>
-      </c>
-      <c r="E128" t="s">
-        <v>34</v>
-      </c>
-      <c r="F128" t="s">
-        <v>37</v>
-      </c>
-      <c r="J128" s="1">
-        <v>1</v>
-      </c>
-      <c r="P128" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="Q128" t="b">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17">
-      <c r="A129" t="s">
-        <v>38</v>
-      </c>
-      <c r="B129" t="str">
-        <f>VLOOKUP(C129,D$127:F$129,3,FALSE)</f>
-        <v>drei</v>
-      </c>
-      <c r="C129" t="s">
-        <v>32</v>
-      </c>
-      <c r="D129" t="s">
-        <v>32</v>
-      </c>
-      <c r="E129" t="s">
-        <v>35</v>
-      </c>
-      <c r="F129" t="s">
-        <v>38</v>
-      </c>
-      <c r="J129" s="1">
-        <v>1</v>
-      </c>
-      <c r="P129" t="b">
-        <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-      <c r="Q129" t="b">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:17">
-      <c r="M130" s="3"/>
-    </row>
-    <row r="131" spans="1:17">
-      <c r="A131">
-        <v>11</v>
-      </c>
-      <c r="B131">
-        <f t="shared" ref="B131:B136" si="17">CHOOSE(C131,D131,E131,F131)</f>
-        <v>11</v>
-      </c>
-      <c r="C131">
-        <v>1</v>
-      </c>
-      <c r="D131">
-        <v>11</v>
-      </c>
-      <c r="E131">
-        <v>12</v>
-      </c>
-      <c r="F131">
-        <v>13</v>
-      </c>
-      <c r="J131" s="1">
-        <v>4</v>
-      </c>
-      <c r="K131" t="s">
-        <v>26</v>
-      </c>
-      <c r="L131" t="s">
-        <v>26</v>
-      </c>
-      <c r="M131" s="3"/>
-      <c r="P131" t="b">
-        <f t="shared" ref="P131:P136" si="18">OR(ISBLANK(B131),IF(ISERROR(B131),ERROR.TYPE(B131)=IF(ISBLANK(M131),ERROR.TYPE(A131),ERROR.TYPE(M131)),IF(ISBLANK(M131),AND(NOT(ISBLANK(A131)),A131=B131),B131=M131)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q131" t="b">
-        <f t="shared" ref="Q131:Q136" si="19">IF(ISBLANK(O131),IF(ISERROR(P131),FALSE,P131),O131)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:17">
-      <c r="A132">
-        <v>22</v>
-      </c>
-      <c r="B132">
-        <f t="shared" si="17"/>
-        <v>22</v>
-      </c>
-      <c r="C132">
-        <v>2</v>
-      </c>
-      <c r="D132">
-        <v>21</v>
-      </c>
-      <c r="E132">
-        <v>22</v>
-      </c>
-      <c r="F132">
-        <v>23</v>
-      </c>
-      <c r="J132" s="1">
-        <v>4</v>
-      </c>
-      <c r="P132" t="b">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="Q132" t="b">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:17">
-      <c r="A133">
-        <v>33</v>
-      </c>
-      <c r="B133">
-        <f t="shared" si="17"/>
-        <v>33</v>
-      </c>
-      <c r="C133">
-        <v>3</v>
-      </c>
-      <c r="D133">
-        <v>31</v>
-      </c>
-      <c r="E133">
-        <v>32</v>
-      </c>
-      <c r="F133">
-        <v>33</v>
-      </c>
-      <c r="J133" s="1">
-        <v>4</v>
-      </c>
       <c r="P133" t="b">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="P133:P141" si="16">OR(ISBLANK(B133),IF(ISERROR(B133),ERROR.TYPE(B133)=IF(ISBLANK(M133),ERROR.TYPE(A133),ERROR.TYPE(M133)),IF(ISBLANK(M133),AND(NOT(ISBLANK(A133)),A133=B133),B133=M133)))</f>
         <v>1</v>
       </c>
       <c r="Q133" t="b">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="Q133:Q141" si="17">IF(ISBLANK(O133),IF(ISERROR(P133),FALSE,P133),O133)</f>
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:17">
       <c r="A134" t="s">
-        <v>28</v>
-      </c>
-      <c r="B134" t="e">
+        <v>34</v>
+      </c>
+      <c r="B134" t="str">
+        <f>VLOOKUP(C134,D$133:F$135,2,FALSE)</f>
+        <v>два</v>
+      </c>
+      <c r="C134" t="s">
+        <v>13</v>
+      </c>
+      <c r="D134" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" t="s">
+        <v>34</v>
+      </c>
+      <c r="F134" t="s">
+        <v>37</v>
+      </c>
+      <c r="J134" s="1">
+        <v>1</v>
+      </c>
+      <c r="P134" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q134" t="b">
         <f t="shared" si="17"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C134">
-        <v>4</v>
-      </c>
-      <c r="D134">
-        <v>11</v>
-      </c>
-      <c r="E134">
-        <v>12</v>
-      </c>
-      <c r="F134">
-        <v>13</v>
-      </c>
-      <c r="J134" s="1">
-        <v>4</v>
-      </c>
-      <c r="M134" s="3" t="e">
-        <v>#VALUE!</v>
-      </c>
-      <c r="P134" t="b">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="Q134" t="b">
-        <f t="shared" si="19"/>
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:17">
       <c r="A135" t="s">
+        <v>38</v>
+      </c>
+      <c r="B135" t="str">
+        <f>VLOOKUP(C135,D$133:F$135,3,FALSE)</f>
+        <v>drei</v>
+      </c>
+      <c r="C135" t="s">
+        <v>32</v>
+      </c>
+      <c r="D135" t="s">
+        <v>32</v>
+      </c>
+      <c r="E135" t="s">
+        <v>35</v>
+      </c>
+      <c r="F135" t="s">
+        <v>38</v>
+      </c>
+      <c r="J135" s="1">
+        <v>1</v>
+      </c>
+      <c r="P135" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q135" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17">
+      <c r="A136" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" t="str">
+        <f t="shared" ref="B136:B141" si="18">VLOOKUP(C136,D$133:F$135,D136,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C136" t="s">
+        <v>12</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="J136" s="1">
+        <v>2</v>
+      </c>
+      <c r="P136" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q136" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17">
+      <c r="A137" t="s">
+        <v>34</v>
+      </c>
+      <c r="B137" t="str">
+        <f t="shared" si="18"/>
+        <v>два</v>
+      </c>
+      <c r="C137" t="s">
+        <v>13</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+      <c r="J137" s="1">
+        <v>2</v>
+      </c>
+      <c r="P137" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q137" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17">
+      <c r="A138" t="s">
+        <v>38</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" si="18"/>
+        <v>drei</v>
+      </c>
+      <c r="C138" t="s">
+        <v>32</v>
+      </c>
+      <c r="D138">
+        <v>3</v>
+      </c>
+      <c r="J138" s="1">
+        <v>2</v>
+      </c>
+      <c r="P138" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q138" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17">
+      <c r="A139" t="s">
+        <v>46</v>
+      </c>
+      <c r="B139" t="e">
+        <f t="shared" si="18"/>
+        <v>#N/A</v>
+      </c>
+      <c r="C139" t="s">
+        <v>40</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="J139" s="1">
+        <v>2</v>
+      </c>
+      <c r="M139" s="3" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P139" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q139" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:17">
+      <c r="A140" t="s">
+        <v>45</v>
+      </c>
+      <c r="B140" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C140" t="s">
+        <v>12</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>2</v>
+      </c>
+      <c r="M140" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P140" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q140" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17">
+      <c r="A141" t="s">
+        <v>45</v>
+      </c>
+      <c r="B141" t="e">
+        <f t="shared" si="18"/>
+        <v>#REF!</v>
+      </c>
+      <c r="C141" t="s">
+        <v>12</v>
+      </c>
+      <c r="D141">
+        <v>4</v>
+      </c>
+      <c r="J141" s="1">
+        <v>2</v>
+      </c>
+      <c r="M141" s="3" t="e">
+        <v>#REF!</v>
+      </c>
+      <c r="P141" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q141" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17">
+      <c r="M142" s="3"/>
+    </row>
+    <row r="143" spans="1:17">
+      <c r="A143">
+        <v>11</v>
+      </c>
+      <c r="B143">
+        <f t="shared" ref="B143:B148" si="19">CHOOSE(C143,D143,E143,F143)</f>
+        <v>11</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>11</v>
+      </c>
+      <c r="E143">
+        <v>12</v>
+      </c>
+      <c r="F143">
+        <v>13</v>
+      </c>
+      <c r="J143" s="1">
+        <v>4</v>
+      </c>
+      <c r="K143" t="s">
+        <v>26</v>
+      </c>
+      <c r="L143" t="s">
+        <v>26</v>
+      </c>
+      <c r="M143" s="3"/>
+      <c r="P143" t="b">
+        <f t="shared" ref="P143:P148" si="20">OR(ISBLANK(B143),IF(ISERROR(B143),ERROR.TYPE(B143)=IF(ISBLANK(M143),ERROR.TYPE(A143),ERROR.TYPE(M143)),IF(ISBLANK(M143),AND(NOT(ISBLANK(A143)),A143=B143),B143=M143)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q143" t="b">
+        <f t="shared" ref="Q143:Q148" si="21">IF(ISBLANK(O143),IF(ISERROR(P143),FALSE,P143),O143)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17">
+      <c r="A144">
+        <v>22</v>
+      </c>
+      <c r="B144">
+        <f t="shared" si="19"/>
+        <v>22</v>
+      </c>
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144">
+        <v>21</v>
+      </c>
+      <c r="E144">
+        <v>22</v>
+      </c>
+      <c r="F144">
+        <v>23</v>
+      </c>
+      <c r="J144" s="1">
+        <v>4</v>
+      </c>
+      <c r="P144" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q144" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17">
+      <c r="A145">
+        <v>33</v>
+      </c>
+      <c r="B145">
+        <f t="shared" si="19"/>
+        <v>33</v>
+      </c>
+      <c r="C145">
+        <v>3</v>
+      </c>
+      <c r="D145">
+        <v>31</v>
+      </c>
+      <c r="E145">
+        <v>32</v>
+      </c>
+      <c r="F145">
+        <v>33</v>
+      </c>
+      <c r="J145" s="1">
+        <v>4</v>
+      </c>
+      <c r="P145" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q145" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17">
+      <c r="A146" t="s">
         <v>28</v>
       </c>
-      <c r="B135" t="e">
-        <f t="shared" si="17"/>
+      <c r="B146" t="e">
+        <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C135">
+      <c r="C146">
+        <v>4</v>
+      </c>
+      <c r="D146">
+        <v>11</v>
+      </c>
+      <c r="E146">
+        <v>12</v>
+      </c>
+      <c r="F146">
+        <v>13</v>
+      </c>
+      <c r="J146" s="1">
+        <v>4</v>
+      </c>
+      <c r="M146" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P146" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q146" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17">
+      <c r="A147" t="s">
+        <v>28</v>
+      </c>
+      <c r="B147" t="e">
+        <f t="shared" si="19"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C147">
         <v>0</v>
       </c>
-      <c r="D135">
+      <c r="D147">
         <v>11</v>
       </c>
-      <c r="E135">
-        <v>12</v>
-      </c>
-      <c r="F135">
+      <c r="E147">
+        <v>12</v>
+      </c>
+      <c r="F147">
         <v>13</v>
       </c>
-      <c r="J135" s="1">
-        <v>4</v>
-      </c>
-      <c r="M135" s="3" t="e">
+      <c r="J147" s="1">
+        <v>4</v>
+      </c>
+      <c r="M147" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P135" t="b">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="Q135" t="b">
+      <c r="P147" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q147" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17">
+      <c r="A148">
+        <v>12</v>
+      </c>
+      <c r="B148">
         <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:17">
-      <c r="A136">
-        <v>12</v>
-      </c>
-      <c r="B136">
-        <f t="shared" si="17"/>
-        <v>12</v>
-      </c>
-      <c r="C136">
+        <v>12</v>
+      </c>
+      <c r="C148">
         <v>2.99</v>
       </c>
-      <c r="D136">
+      <c r="D148">
         <v>11</v>
       </c>
-      <c r="E136">
-        <v>12</v>
-      </c>
-      <c r="F136">
+      <c r="E148">
+        <v>12</v>
+      </c>
+      <c r="F148">
         <v>13</v>
       </c>
-      <c r="J136" s="1">
-        <v>4</v>
-      </c>
-      <c r="P136" t="b">
-        <f t="shared" si="18"/>
-        <v>1</v>
-      </c>
-      <c r="Q136" t="b">
-        <f t="shared" si="19"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="13:13">
-      <c r="M150" s="3"/>
-    </row>
-    <row r="154" spans="13:13">
-      <c r="M154" s="3"/>
-    </row>
-    <row r="156" spans="13:13">
-      <c r="M156" s="3"/>
-    </row>
-    <row r="157" spans="13:13">
-      <c r="M157" s="3"/>
-    </row>
-    <row r="159" spans="13:13">
-      <c r="M159" s="3"/>
-    </row>
-    <row r="161" spans="13:13">
-      <c r="M161" s="3"/>
+      <c r="J148" s="1">
+        <v>4</v>
+      </c>
+      <c r="P148" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q148" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="162" spans="13:13">
       <c r="M162" s="3"/>
@@ -4200,39 +4535,21 @@
     <row r="166" spans="13:13">
       <c r="M166" s="3"/>
     </row>
-    <row r="167" spans="13:13">
-      <c r="M167" s="3"/>
-    </row>
     <row r="168" spans="13:13">
       <c r="M168" s="3"/>
     </row>
     <row r="169" spans="13:13">
       <c r="M169" s="3"/>
     </row>
-    <row r="170" spans="13:13">
-      <c r="M170" s="3"/>
-    </row>
     <row r="171" spans="13:13">
       <c r="M171" s="3"/>
     </row>
-    <row r="172" spans="13:13">
-      <c r="M172" s="3"/>
-    </row>
     <row r="173" spans="13:13">
       <c r="M173" s="3"/>
     </row>
     <row r="174" spans="13:13">
       <c r="M174" s="3"/>
     </row>
-    <row r="175" spans="13:13">
-      <c r="M175" s="3"/>
-    </row>
-    <row r="176" spans="13:13">
-      <c r="M176" s="3"/>
-    </row>
-    <row r="177" spans="13:13">
-      <c r="M177" s="3"/>
-    </row>
     <row r="178" spans="13:13">
       <c r="M178" s="3"/>
     </row>
@@ -4263,23 +4580,59 @@
     <row r="187" spans="13:13">
       <c r="M187" s="3"/>
     </row>
+    <row r="188" spans="13:13">
+      <c r="M188" s="3"/>
+    </row>
+    <row r="189" spans="13:13">
+      <c r="M189" s="3"/>
+    </row>
+    <row r="190" spans="13:13">
+      <c r="M190" s="3"/>
+    </row>
+    <row r="191" spans="13:13">
+      <c r="M191" s="3"/>
+    </row>
+    <row r="192" spans="13:13">
+      <c r="M192" s="3"/>
+    </row>
+    <row r="193" spans="13:13">
+      <c r="M193" s="3"/>
+    </row>
+    <row r="194" spans="13:13">
+      <c r="M194" s="3"/>
+    </row>
+    <row r="195" spans="13:13">
+      <c r="M195" s="3"/>
+    </row>
+    <row r="196" spans="13:13">
+      <c r="M196" s="3"/>
+    </row>
+    <row r="197" spans="13:13">
+      <c r="M197" s="3"/>
+    </row>
+    <row r="198" spans="13:13">
+      <c r="M198" s="3"/>
+    </row>
+    <row r="199" spans="13:13">
+      <c r="M199" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A10017">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A2:A10029">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I10017">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="C2:I10029">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M10017">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="M2:M10029">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Implement ROW and COLUMN.
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
   <si>
     <t>Actual</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>!STR:NA</t>
+  </si>
+  <si>
+    <t>COLUMN</t>
+  </si>
+  <si>
+    <t>ROW</t>
   </si>
 </sst>
 </file>
@@ -213,21 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="27"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor indexed="29"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -4529,6 +4521,98 @@
         <v>1</v>
       </c>
     </row>
+    <row r="150" spans="1:17">
+      <c r="A150">
+        <v>2</v>
+      </c>
+      <c r="B150">
+        <f>COLUMN()</f>
+        <v>2</v>
+      </c>
+      <c r="J150" s="1">
+        <v>0</v>
+      </c>
+      <c r="K150" t="s">
+        <v>47</v>
+      </c>
+      <c r="L150" t="s">
+        <v>47</v>
+      </c>
+      <c r="P150" t="b">
+        <f t="shared" ref="P150:P151" si="22">OR(ISBLANK(B150),IF(ISERROR(B150),ERROR.TYPE(B150)=IF(ISBLANK(M150),ERROR.TYPE(A150),ERROR.TYPE(M150)),IF(ISBLANK(M150),AND(NOT(ISBLANK(A150)),A150=B150),B150=M150)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q150" t="b">
+        <f t="shared" ref="Q150:Q151" si="23">IF(ISBLANK(O150),IF(ISERROR(P150),FALSE,P150),O150)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17">
+      <c r="A151">
+        <v>3</v>
+      </c>
+      <c r="B151">
+        <f>COLUMN(C151)</f>
+        <v>3</v>
+      </c>
+      <c r="J151" s="1">
+        <v>1</v>
+      </c>
+      <c r="P151" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="Q151" t="b">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17">
+      <c r="A153">
+        <v>153</v>
+      </c>
+      <c r="B153">
+        <f>ROW()</f>
+        <v>153</v>
+      </c>
+      <c r="J153" s="1">
+        <v>0</v>
+      </c>
+      <c r="K153" t="s">
+        <v>48</v>
+      </c>
+      <c r="L153" t="s">
+        <v>48</v>
+      </c>
+      <c r="P153" t="b">
+        <f t="shared" ref="P153:P154" si="24">OR(ISBLANK(B153),IF(ISERROR(B153),ERROR.TYPE(B153)=IF(ISBLANK(M153),ERROR.TYPE(A153),ERROR.TYPE(M153)),IF(ISBLANK(M153),AND(NOT(ISBLANK(A153)),A153=B153),B153=M153)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q153" t="b">
+        <f t="shared" ref="Q153:Q154" si="25">IF(ISBLANK(O153),IF(ISERROR(P153),FALSE,P153),O153)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17">
+      <c r="A154">
+        <v>154</v>
+      </c>
+      <c r="B154">
+        <f>ROW(C154)</f>
+        <v>154</v>
+      </c>
+      <c r="J154" s="1">
+        <v>1</v>
+      </c>
+      <c r="P154" t="b">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="Q154" t="b">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+    </row>
     <row r="162" spans="13:13">
       <c r="M162" s="3"/>
     </row>
@@ -4619,20 +4703,20 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10029">
-    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I10029">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M10029">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
compiler: fix bug with nested calls to INDEX (issue 28)
Compiler used to use the same internal method name for the indexer method.
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="50">
   <si>
     <t>Actual</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>ROW</t>
+  </si>
+  <si>
+    <t>INDEX (nested)</t>
   </si>
 </sst>
 </file>
@@ -219,7 +222,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -538,9 +597,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q199"/>
+  <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -2657,41 +2718,38 @@
     </row>
     <row r="82" spans="1:17">
       <c r="A82">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B82">
-        <f>LOOKUP(C82,D82:F82,G82:I82)</f>
-        <v>12</v>
+        <f>INDEX(F82:G82,H82)</f>
+        <v>2</v>
       </c>
       <c r="C82">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D82">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F82">
-        <v>30</v>
+        <f>INDEX(C82:D82,E82)</f>
+        <v>1</v>
       </c>
       <c r="G82">
-        <v>11</v>
+        <f>INDEX(E82:E82,D82)</f>
+        <v>2</v>
       </c>
       <c r="H82">
-        <v>12</v>
-      </c>
-      <c r="I82">
-        <v>13</v>
+        <f>INDEX(D82:E82,C82)</f>
+        <v>2</v>
       </c>
       <c r="J82" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K82" t="s">
-        <v>19</v>
-      </c>
-      <c r="L82" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="P82" t="b">
         <f>OR(ISBLANK(B82),IF(ISERROR(B82),ERROR.TYPE(B82)=IF(ISBLANK(M82),ERROR.TYPE(A82),ERROR.TYPE(M82)),IF(ISBLANK(M82),AND(NOT(ISBLANK(A82)),A82=B82),B82=M82)))</f>
@@ -2702,47 +2760,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:17">
-      <c r="A83">
-        <v>11</v>
-      </c>
-      <c r="B83">
-        <f>LOOKUP(C83,D83:F83,G83:I83)</f>
-        <v>11</v>
-      </c>
-      <c r="C83">
-        <v>19</v>
-      </c>
-      <c r="D83">
-        <v>10</v>
-      </c>
-      <c r="E83">
-        <v>20</v>
-      </c>
-      <c r="F83">
-        <v>30</v>
-      </c>
-      <c r="G83">
-        <v>11</v>
-      </c>
-      <c r="H83">
-        <v>12</v>
-      </c>
-      <c r="I83">
-        <v>13</v>
-      </c>
-      <c r="J83" s="1">
-        <v>7</v>
-      </c>
-      <c r="P83" t="b">
-        <f>OR(ISBLANK(B83),IF(ISERROR(B83),ERROR.TYPE(B83)=IF(ISBLANK(M83),ERROR.TYPE(A83),ERROR.TYPE(M83)),IF(ISBLANK(M83),AND(NOT(ISBLANK(A83)),A83=B83),B83=M83)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q83" t="b">
-        <f>IF(ISBLANK(O83),IF(ISERROR(P83),FALSE,P83),O83)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="84" spans="1:17">
       <c r="A84">
         <v>12</v>
@@ -2752,7 +2769,7 @@
         <v>12</v>
       </c>
       <c r="C84">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D84">
         <v>10</v>
@@ -2775,6 +2792,12 @@
       <c r="J84" s="1">
         <v>7</v>
       </c>
+      <c r="K84" t="s">
+        <v>19</v>
+      </c>
+      <c r="L84" t="s">
+        <v>15</v>
+      </c>
       <c r="P84" t="b">
         <f>OR(ISBLANK(B84),IF(ISERROR(B84),ERROR.TYPE(B84)=IF(ISBLANK(M84),ERROR.TYPE(A84),ERROR.TYPE(M84)),IF(ISBLANK(M84),AND(NOT(ISBLANK(A84)),A84=B84),B84=M84)))</f>
         <v>1</v>
@@ -2785,15 +2808,15 @@
       </c>
     </row>
     <row r="85" spans="1:17">
-      <c r="A85" t="s">
-        <v>27</v>
-      </c>
-      <c r="B85" t="e">
+      <c r="A85">
+        <v>11</v>
+      </c>
+      <c r="B85">
         <f>LOOKUP(C85,D85:F85,G85:I85)</f>
-        <v>#N/A</v>
+        <v>11</v>
       </c>
       <c r="C85">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D85">
         <v>10</v>
@@ -2816,9 +2839,6 @@
       <c r="J85" s="1">
         <v>7</v>
       </c>
-      <c r="M85" s="3" t="e">
-        <v>#N/A</v>
-      </c>
       <c r="P85" t="b">
         <f>OR(ISBLANK(B85),IF(ISERROR(B85),ERROR.TYPE(B85)=IF(ISBLANK(M85),ERROR.TYPE(A85),ERROR.TYPE(M85)),IF(ISBLANK(M85),AND(NOT(ISBLANK(A85)),A85=B85),B85=M85)))</f>
         <v>1</v>
@@ -2828,28 +2848,81 @@
         <v>1</v>
       </c>
     </row>
+    <row r="86" spans="1:17">
+      <c r="A86">
+        <v>12</v>
+      </c>
+      <c r="B86">
+        <f>LOOKUP(C86,D86:F86,G86:I86)</f>
+        <v>12</v>
+      </c>
+      <c r="C86">
+        <v>21</v>
+      </c>
+      <c r="D86">
+        <v>10</v>
+      </c>
+      <c r="E86">
+        <v>20</v>
+      </c>
+      <c r="F86">
+        <v>30</v>
+      </c>
+      <c r="G86">
+        <v>11</v>
+      </c>
+      <c r="H86">
+        <v>12</v>
+      </c>
+      <c r="I86">
+        <v>13</v>
+      </c>
+      <c r="J86" s="1">
+        <v>7</v>
+      </c>
+      <c r="P86" t="b">
+        <f>OR(ISBLANK(B86),IF(ISERROR(B86),ERROR.TYPE(B86)=IF(ISBLANK(M86),ERROR.TYPE(A86),ERROR.TYPE(M86)),IF(ISBLANK(M86),AND(NOT(ISBLANK(A86)),A86=B86),B86=M86)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q86" t="b">
+        <f>IF(ISBLANK(O86),IF(ISERROR(P86),FALSE,P86),O86)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="87" spans="1:17">
-      <c r="A87">
-        <v>11</v>
-      </c>
-      <c r="B87">
-        <f>LOOKUP(C87,D$87:D$89,E$87:E$89)</f>
-        <v>11</v>
+      <c r="A87" t="s">
+        <v>27</v>
+      </c>
+      <c r="B87" t="e">
+        <f>LOOKUP(C87,D87:F87,G87:I87)</f>
+        <v>#N/A</v>
       </c>
       <c r="C87">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D87">
         <v>10</v>
       </c>
       <c r="E87">
+        <v>20</v>
+      </c>
+      <c r="F87">
+        <v>30</v>
+      </c>
+      <c r="G87">
         <v>11</v>
       </c>
+      <c r="H87">
+        <v>12</v>
+      </c>
+      <c r="I87">
+        <v>13</v>
+      </c>
       <c r="J87" s="1">
-        <v>3</v>
-      </c>
-      <c r="K87" t="s">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="M87" s="3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="P87" t="b">
         <f>OR(ISBLANK(B87),IF(ISERROR(B87),ERROR.TYPE(B87)=IF(ISBLANK(M87),ERROR.TYPE(A87),ERROR.TYPE(M87)),IF(ISBLANK(M87),AND(NOT(ISBLANK(A87)),A87=B87),B87=M87)))</f>
@@ -2860,54 +2933,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:17">
-      <c r="A88">
-        <v>12</v>
-      </c>
-      <c r="B88">
-        <f>LOOKUP(C88,D$87:D$89,E$87:E$89)</f>
-        <v>12</v>
-      </c>
-      <c r="C88">
-        <v>20</v>
-      </c>
-      <c r="D88">
-        <v>20</v>
-      </c>
-      <c r="E88">
-        <v>12</v>
-      </c>
-      <c r="J88" s="1">
-        <v>1</v>
-      </c>
-      <c r="P88" t="b">
-        <f>OR(ISBLANK(B88),IF(ISERROR(B88),ERROR.TYPE(B88)=IF(ISBLANK(M88),ERROR.TYPE(A88),ERROR.TYPE(M88)),IF(ISBLANK(M88),AND(NOT(ISBLANK(A88)),A88=B88),B88=M88)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q88" t="b">
-        <f>IF(ISBLANK(O88),IF(ISERROR(P88),FALSE,P88),O88)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="89" spans="1:17">
       <c r="A89">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B89">
-        <f>LOOKUP(C89,D$87:D$89,E$87:E$89)</f>
-        <v>12</v>
+        <f>LOOKUP(C89,D$89:D$91,E$89:E$91)</f>
+        <v>11</v>
       </c>
       <c r="C89">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D89">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E89">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J89" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="K89" t="s">
+        <v>20</v>
       </c>
       <c r="P89" t="b">
         <f>OR(ISBLANK(B89),IF(ISERROR(B89),ERROR.TYPE(B89)=IF(ISBLANK(M89),ERROR.TYPE(A89),ERROR.TYPE(M89)),IF(ISBLANK(M89),AND(NOT(ISBLANK(A89)),A89=B89),B89=M89)))</f>
@@ -2919,21 +2966,24 @@
       </c>
     </row>
     <row r="90" spans="1:17">
-      <c r="A90" t="s">
-        <v>27</v>
-      </c>
-      <c r="B90" t="e">
-        <f>LOOKUP(C90,D$87:D$89,E$87:E$89)</f>
-        <v>#N/A</v>
+      <c r="A90">
+        <v>12</v>
+      </c>
+      <c r="B90">
+        <f>LOOKUP(C90,D$89:D$91,E$89:E$91)</f>
+        <v>12</v>
       </c>
       <c r="C90">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="D90">
+        <v>20</v>
+      </c>
+      <c r="E90">
+        <v>12</v>
       </c>
       <c r="J90" s="1">
         <v>1</v>
-      </c>
-      <c r="M90" s="3" t="e">
-        <v>#N/A</v>
       </c>
       <c r="P90" t="b">
         <f>OR(ISBLANK(B90),IF(ISERROR(B90),ERROR.TYPE(B90)=IF(ISBLANK(M90),ERROR.TYPE(A90),ERROR.TYPE(M90)),IF(ISBLANK(M90),AND(NOT(ISBLANK(A90)),A90=B90),B90=M90)))</f>
@@ -2944,34 +2994,51 @@
         <v>1</v>
       </c>
     </row>
+    <row r="91" spans="1:17">
+      <c r="A91">
+        <v>12</v>
+      </c>
+      <c r="B91">
+        <f>LOOKUP(C91,D$89:D$91,E$89:E$91)</f>
+        <v>12</v>
+      </c>
+      <c r="C91">
+        <v>21</v>
+      </c>
+      <c r="D91">
+        <v>30</v>
+      </c>
+      <c r="E91">
+        <v>13</v>
+      </c>
+      <c r="J91" s="1">
+        <v>1</v>
+      </c>
+      <c r="P91" t="b">
+        <f>OR(ISBLANK(B91),IF(ISERROR(B91),ERROR.TYPE(B91)=IF(ISBLANK(M91),ERROR.TYPE(A91),ERROR.TYPE(M91)),IF(ISBLANK(M91),AND(NOT(ISBLANK(A91)),A91=B91),B91=M91)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q91" t="b">
+        <f>IF(ISBLANK(O91),IF(ISERROR(P91),FALSE,P91),O91)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="92" spans="1:17">
-      <c r="A92">
-        <v>22</v>
-      </c>
-      <c r="B92">
-        <f>LOOKUP(C92,D$92:G$94)</f>
-        <v>22</v>
+      <c r="A92" t="s">
+        <v>27</v>
+      </c>
+      <c r="B92" t="e">
+        <f>LOOKUP(C92,D$89:D$91,E$89:E$91)</f>
+        <v>#N/A</v>
       </c>
       <c r="C92">
-        <v>29</v>
-      </c>
-      <c r="D92">
-        <v>10</v>
-      </c>
-      <c r="E92">
-        <v>20</v>
-      </c>
-      <c r="F92">
-        <v>30</v>
-      </c>
-      <c r="G92">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="J92" s="1">
-        <v>5</v>
-      </c>
-      <c r="K92" t="s">
-        <v>16</v>
+        <v>1</v>
+      </c>
+      <c r="M92" s="3" t="e">
+        <v>#N/A</v>
       </c>
       <c r="P92" t="b">
         <f>OR(ISBLANK(B92),IF(ISERROR(B92),ERROR.TYPE(B92)=IF(ISBLANK(M92),ERROR.TYPE(A92),ERROR.TYPE(M92)),IF(ISBLANK(M92),AND(NOT(ISBLANK(A92)),A92=B92),B92=M92)))</f>
@@ -2982,66 +3049,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:17">
-      <c r="A93">
-        <v>23</v>
-      </c>
-      <c r="B93">
-        <f>LOOKUP(C93,D$92:G$94)</f>
-        <v>23</v>
-      </c>
-      <c r="C93">
-        <v>30</v>
-      </c>
-      <c r="D93">
-        <v>11</v>
-      </c>
-      <c r="E93">
-        <v>12</v>
-      </c>
-      <c r="F93">
-        <v>13</v>
-      </c>
-      <c r="G93">
-        <v>14</v>
-      </c>
-      <c r="J93" s="1">
-        <v>1</v>
-      </c>
-      <c r="P93" t="b">
-        <f>OR(ISBLANK(B93),IF(ISERROR(B93),ERROR.TYPE(B93)=IF(ISBLANK(M93),ERROR.TYPE(A93),ERROR.TYPE(M93)),IF(ISBLANK(M93),AND(NOT(ISBLANK(A93)),A93=B93),B93=M93)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q93" t="b">
-        <f>IF(ISBLANK(O93),IF(ISERROR(P93),FALSE,P93),O93)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="94" spans="1:17">
       <c r="A94">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B94">
-        <f>LOOKUP(C94,D$92:G$94)</f>
-        <v>23</v>
+        <f>LOOKUP(C94,D$94:G$96)</f>
+        <v>22</v>
       </c>
       <c r="C94">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D94">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E94">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F94">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G94">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="J94" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="K94" t="s">
+        <v>16</v>
       </c>
       <c r="P94" t="b">
         <f>OR(ISBLANK(B94),IF(ISERROR(B94),ERROR.TYPE(B94)=IF(ISBLANK(M94),ERROR.TYPE(A94),ERROR.TYPE(M94)),IF(ISBLANK(M94),AND(NOT(ISBLANK(A94)),A94=B94),B94=M94)))</f>
@@ -3052,31 +3087,66 @@
         <v>1</v>
       </c>
     </row>
+    <row r="95" spans="1:17">
+      <c r="A95">
+        <v>23</v>
+      </c>
+      <c r="B95">
+        <f>LOOKUP(C95,D$94:G$96)</f>
+        <v>23</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+      <c r="D95">
+        <v>11</v>
+      </c>
+      <c r="E95">
+        <v>12</v>
+      </c>
+      <c r="F95">
+        <v>13</v>
+      </c>
+      <c r="G95">
+        <v>14</v>
+      </c>
+      <c r="J95" s="1">
+        <v>1</v>
+      </c>
+      <c r="P95" t="b">
+        <f>OR(ISBLANK(B95),IF(ISERROR(B95),ERROR.TYPE(B95)=IF(ISBLANK(M95),ERROR.TYPE(A95),ERROR.TYPE(M95)),IF(ISBLANK(M95),AND(NOT(ISBLANK(A95)),A95=B95),B95=M95)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q95" t="b">
+        <f>IF(ISBLANK(O95),IF(ISERROR(P95),FALSE,P95),O95)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="96" spans="1:17">
       <c r="A96">
+        <v>23</v>
+      </c>
+      <c r="B96">
+        <f>LOOKUP(C96,D$94:G$96)</f>
+        <v>23</v>
+      </c>
+      <c r="C96">
+        <v>31</v>
+      </c>
+      <c r="D96">
         <v>21</v>
       </c>
-      <c r="B96">
-        <f>LOOKUP(C96,D$96:F$98)</f>
-        <v>21</v>
-      </c>
-      <c r="C96">
-        <v>19</v>
-      </c>
-      <c r="D96">
-        <v>10</v>
-      </c>
       <c r="E96">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F96">
-        <v>21</v>
+        <v>23</v>
+      </c>
+      <c r="G96">
+        <v>24</v>
       </c>
       <c r="J96" s="1">
-        <v>4</v>
-      </c>
-      <c r="K96" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="P96" t="b">
         <f>OR(ISBLANK(B96),IF(ISERROR(B96),ERROR.TYPE(B96)=IF(ISBLANK(M96),ERROR.TYPE(A96),ERROR.TYPE(M96)),IF(ISBLANK(M96),AND(NOT(ISBLANK(A96)),A96=B96),B96=M96)))</f>
@@ -3087,60 +3157,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
-      <c r="A97">
-        <v>22</v>
-      </c>
-      <c r="B97">
-        <f>LOOKUP(C97,D$96:F$98)</f>
-        <v>22</v>
-      </c>
-      <c r="C97">
-        <v>20</v>
-      </c>
-      <c r="D97">
-        <v>20</v>
-      </c>
-      <c r="E97">
-        <v>12</v>
-      </c>
-      <c r="F97">
-        <v>22</v>
-      </c>
-      <c r="J97" s="1">
-        <v>1</v>
-      </c>
-      <c r="P97" t="b">
-        <f>OR(ISBLANK(B97),IF(ISERROR(B97),ERROR.TYPE(B97)=IF(ISBLANK(M97),ERROR.TYPE(A97),ERROR.TYPE(M97)),IF(ISBLANK(M97),AND(NOT(ISBLANK(A97)),A97=B97),B97=M97)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q97" t="b">
-        <f>IF(ISBLANK(O97),IF(ISERROR(P97),FALSE,P97),O97)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="98" spans="1:17">
       <c r="A98">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B98">
-        <f>LOOKUP(C98,D$96:F$98)</f>
-        <v>22</v>
+        <f>LOOKUP(C98,D$98:F$100)</f>
+        <v>21</v>
       </c>
       <c r="C98">
+        <v>19</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98">
+        <v>11</v>
+      </c>
+      <c r="F98">
         <v>21</v>
       </c>
-      <c r="D98">
-        <v>30</v>
-      </c>
-      <c r="E98">
-        <v>13</v>
-      </c>
-      <c r="F98">
-        <v>23</v>
-      </c>
       <c r="J98" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K98" t="s">
+        <v>18</v>
       </c>
       <c r="P98" t="b">
         <f>OR(ISBLANK(B98),IF(ISERROR(B98),ERROR.TYPE(B98)=IF(ISBLANK(M98),ERROR.TYPE(A98),ERROR.TYPE(M98)),IF(ISBLANK(M98),AND(NOT(ISBLANK(A98)),A98=B98),B98=M98)))</f>
@@ -3151,31 +3192,60 @@
         <v>1</v>
       </c>
     </row>
+    <row r="99" spans="1:17">
+      <c r="A99">
+        <v>22</v>
+      </c>
+      <c r="B99">
+        <f>LOOKUP(C99,D$98:F$100)</f>
+        <v>22</v>
+      </c>
+      <c r="C99">
+        <v>20</v>
+      </c>
+      <c r="D99">
+        <v>20</v>
+      </c>
+      <c r="E99">
+        <v>12</v>
+      </c>
+      <c r="F99">
+        <v>22</v>
+      </c>
+      <c r="J99" s="1">
+        <v>1</v>
+      </c>
+      <c r="P99" t="b">
+        <f>OR(ISBLANK(B99),IF(ISERROR(B99),ERROR.TYPE(B99)=IF(ISBLANK(M99),ERROR.TYPE(A99),ERROR.TYPE(M99)),IF(ISBLANK(M99),AND(NOT(ISBLANK(A99)),A99=B99),B99=M99)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q99" t="b">
+        <f>IF(ISBLANK(O99),IF(ISERROR(P99),FALSE,P99),O99)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="100" spans="1:17">
       <c r="A100">
+        <v>22</v>
+      </c>
+      <c r="B100">
+        <f>LOOKUP(C100,D$98:F$100)</f>
+        <v>22</v>
+      </c>
+      <c r="C100">
         <v>21</v>
       </c>
-      <c r="B100">
-        <f>LOOKUP(C100,D$100:F$103)</f>
-        <v>21</v>
-      </c>
-      <c r="C100">
-        <v>19</v>
-      </c>
       <c r="D100">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="E100">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F100">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J100" s="1">
-        <v>4</v>
-      </c>
-      <c r="K100" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="P100" t="b">
         <f>OR(ISBLANK(B100),IF(ISERROR(B100),ERROR.TYPE(B100)=IF(ISBLANK(M100),ERROR.TYPE(A100),ERROR.TYPE(M100)),IF(ISBLANK(M100),AND(NOT(ISBLANK(A100)),A100=B100),B100=M100)))</f>
@@ -3186,60 +3256,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
-      <c r="A101">
-        <v>22</v>
-      </c>
-      <c r="B101">
-        <f>LOOKUP(C101,D$100:F$103)</f>
-        <v>22</v>
-      </c>
-      <c r="C101">
-        <v>20</v>
-      </c>
-      <c r="D101">
-        <v>20</v>
-      </c>
-      <c r="E101">
-        <v>12</v>
-      </c>
-      <c r="F101">
-        <v>22</v>
-      </c>
-      <c r="J101" s="1">
-        <v>1</v>
-      </c>
-      <c r="P101" t="b">
-        <f>OR(ISBLANK(B101),IF(ISERROR(B101),ERROR.TYPE(B101)=IF(ISBLANK(M101),ERROR.TYPE(A101),ERROR.TYPE(M101)),IF(ISBLANK(M101),AND(NOT(ISBLANK(A101)),A101=B101),B101=M101)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q101" t="b">
-        <f>IF(ISBLANK(O101),IF(ISERROR(P101),FALSE,P101),O101)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="102" spans="1:17">
       <c r="A102">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B102">
-        <f>LOOKUP(C102,D$100:F$103)</f>
-        <v>22</v>
+        <f>LOOKUP(C102,D$102:F$105)</f>
+        <v>21</v>
       </c>
       <c r="C102">
+        <v>19</v>
+      </c>
+      <c r="D102">
+        <v>10</v>
+      </c>
+      <c r="E102">
+        <v>11</v>
+      </c>
+      <c r="F102">
         <v>21</v>
       </c>
-      <c r="D102">
-        <v>30</v>
-      </c>
-      <c r="E102">
-        <v>13</v>
-      </c>
-      <c r="F102">
-        <v>23</v>
-      </c>
       <c r="J102" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K102" t="s">
+        <v>17</v>
       </c>
       <c r="P102" t="b">
         <f>OR(ISBLANK(B102),IF(ISERROR(B102),ERROR.TYPE(B102)=IF(ISBLANK(M102),ERROR.TYPE(A102),ERROR.TYPE(M102)),IF(ISBLANK(M102),AND(NOT(ISBLANK(A102)),A102=B102),B102=M102)))</f>
@@ -3252,23 +3293,23 @@
     </row>
     <row r="103" spans="1:17">
       <c r="A103">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B103">
-        <f>LOOKUP(C103,D$100:F$103)</f>
-        <v>23</v>
+        <f>LOOKUP(C103,D$102:F$105)</f>
+        <v>22</v>
       </c>
       <c r="C103">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D103">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="E103">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F103">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J103" s="1">
         <v>1</v>
@@ -3282,133 +3323,136 @@
         <v>1</v>
       </c>
     </row>
+    <row r="104" spans="1:17">
+      <c r="A104">
+        <v>22</v>
+      </c>
+      <c r="B104">
+        <f>LOOKUP(C104,D$102:F$105)</f>
+        <v>22</v>
+      </c>
+      <c r="C104">
+        <v>21</v>
+      </c>
+      <c r="D104">
+        <v>30</v>
+      </c>
+      <c r="E104">
+        <v>13</v>
+      </c>
+      <c r="F104">
+        <v>23</v>
+      </c>
+      <c r="J104" s="1">
+        <v>1</v>
+      </c>
+      <c r="P104" t="b">
+        <f>OR(ISBLANK(B104),IF(ISERROR(B104),ERROR.TYPE(B104)=IF(ISBLANK(M104),ERROR.TYPE(A104),ERROR.TYPE(M104)),IF(ISBLANK(M104),AND(NOT(ISBLANK(A104)),A104=B104),B104=M104)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q104" t="b">
+        <f>IF(ISBLANK(O104),IF(ISERROR(P104),FALSE,P104),O104)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="105" spans="1:17">
       <c r="A105">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B105">
-        <f>HLOOKUP(C105,D$105:G$107,3)</f>
-        <v>22</v>
+        <f>LOOKUP(C105,D$102:F$105)</f>
+        <v>23</v>
       </c>
       <c r="C105">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D105">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E105">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="F105">
-        <v>30</v>
-      </c>
-      <c r="G105">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="J105" s="1">
-        <v>5</v>
-      </c>
-      <c r="K105" t="s">
-        <v>24</v>
-      </c>
-      <c r="L105" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="P105" t="b">
-        <f t="shared" ref="P105:P112" si="9">OR(ISBLANK(B105),IF(ISERROR(B105),ERROR.TYPE(B105)=IF(ISBLANK(M105),ERROR.TYPE(A105),ERROR.TYPE(M105)),IF(ISBLANK(M105),AND(NOT(ISBLANK(A105)),A105=B105),B105=M105)))</f>
+        <f>OR(ISBLANK(B105),IF(ISERROR(B105),ERROR.TYPE(B105)=IF(ISBLANK(M105),ERROR.TYPE(A105),ERROR.TYPE(M105)),IF(ISBLANK(M105),AND(NOT(ISBLANK(A105)),A105=B105),B105=M105)))</f>
         <v>1</v>
       </c>
       <c r="Q105" t="b">
-        <f t="shared" ref="Q105:Q112" si="10">IF(ISBLANK(O105),IF(ISERROR(P105),FALSE,P105),O105)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:17">
-      <c r="A106">
-        <v>23</v>
-      </c>
-      <c r="B106">
-        <f>HLOOKUP(C106,D$105:G$107,3)</f>
-        <v>23</v>
-      </c>
-      <c r="C106">
-        <v>30</v>
-      </c>
-      <c r="D106">
-        <v>11</v>
-      </c>
-      <c r="E106">
-        <v>12</v>
-      </c>
-      <c r="F106">
-        <v>13</v>
-      </c>
-      <c r="G106">
-        <v>14</v>
-      </c>
-      <c r="J106" s="1">
-        <v>1</v>
-      </c>
-      <c r="P106" t="b">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
-      <c r="Q106" t="b">
-        <f t="shared" si="10"/>
+        <f>IF(ISBLANK(O105),IF(ISERROR(P105),FALSE,P105),O105)</f>
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:17">
       <c r="A107">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B107">
-        <f>HLOOKUP(C107,D$105:G$107,3)</f>
-        <v>23</v>
+        <f>HLOOKUP(C107,D$107:G$109,3)</f>
+        <v>22</v>
       </c>
       <c r="C107">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D107">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E107">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F107">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G107">
+        <v>40</v>
+      </c>
+      <c r="J107" s="1">
+        <v>5</v>
+      </c>
+      <c r="K107" t="s">
         <v>24</v>
       </c>
-      <c r="J107" s="1">
-        <v>1</v>
+      <c r="L107" t="s">
+        <v>24</v>
       </c>
       <c r="P107" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="P107:P114" si="9">OR(ISBLANK(B107),IF(ISERROR(B107),ERROR.TYPE(B107)=IF(ISBLANK(M107),ERROR.TYPE(A107),ERROR.TYPE(M107)),IF(ISBLANK(M107),AND(NOT(ISBLANK(A107)),A107=B107),B107=M107)))</f>
         <v>1</v>
       </c>
       <c r="Q107" t="b">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="Q107:Q114" si="10">IF(ISBLANK(O107),IF(ISERROR(P107),FALSE,P107),O107)</f>
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:17">
       <c r="A108">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B108">
-        <f>HLOOKUP(C108,D$105:G$107,D108)</f>
-        <v>20</v>
+        <f>HLOOKUP(C108,D$107:G$109,3)</f>
+        <v>23</v>
       </c>
       <c r="C108">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="E108">
+        <v>12</v>
+      </c>
+      <c r="F108">
+        <v>13</v>
+      </c>
+      <c r="G108">
+        <v>14</v>
       </c>
       <c r="J108" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P108" t="b">
         <f t="shared" si="9"/>
@@ -3421,20 +3465,29 @@
     </row>
     <row r="109" spans="1:17">
       <c r="A109">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B109">
-        <f>HLOOKUP(C109,D$105:G$107,D109)</f>
-        <v>13</v>
+        <f>HLOOKUP(C109,D$107:G$109,3)</f>
+        <v>23</v>
       </c>
       <c r="C109">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D109">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="E109">
+        <v>22</v>
+      </c>
+      <c r="F109">
+        <v>23</v>
+      </c>
+      <c r="G109">
+        <v>24</v>
       </c>
       <c r="J109" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P109" t="b">
         <f t="shared" si="9"/>
@@ -3447,17 +3500,17 @@
     </row>
     <row r="110" spans="1:17">
       <c r="A110">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B110">
-        <f>HLOOKUP(C110,D$105:G$107,D110)</f>
-        <v>23</v>
+        <f>HLOOKUP(C110,D$107:G$109,D110)</f>
+        <v>20</v>
       </c>
       <c r="C110">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D110">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J110" s="1">
         <v>2</v>
@@ -3472,24 +3525,21 @@
       </c>
     </row>
     <row r="111" spans="1:17">
-      <c r="A111" t="s">
-        <v>28</v>
-      </c>
-      <c r="B111" t="e">
-        <f>HLOOKUP(C111,D$105:G$107,D111)</f>
-        <v>#VALUE!</v>
+      <c r="A111">
+        <v>13</v>
+      </c>
+      <c r="B111">
+        <f>HLOOKUP(C111,D$107:G$109,D111)</f>
+        <v>13</v>
       </c>
       <c r="C111">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J111" s="1">
         <v>2</v>
-      </c>
-      <c r="M111" s="3" t="e">
-        <v>#VALUE!</v>
       </c>
       <c r="P111" t="b">
         <f t="shared" si="9"/>
@@ -3501,24 +3551,21 @@
       </c>
     </row>
     <row r="112" spans="1:17">
-      <c r="A112" t="s">
-        <v>28</v>
-      </c>
-      <c r="B112" t="e">
-        <f>HLOOKUP(C112,D$105:G$107,D112)</f>
-        <v>#REF!</v>
+      <c r="A112">
+        <v>23</v>
+      </c>
+      <c r="B112">
+        <f>HLOOKUP(C112,D$107:G$109,D112)</f>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>31</v>
       </c>
       <c r="D112">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J112" s="1">
         <v>2</v>
-      </c>
-      <c r="M112" s="3" t="e">
-        <v>#REF!</v>
       </c>
       <c r="P112" t="b">
         <f t="shared" si="9"/>
@@ -3529,133 +3576,130 @@
         <v>1</v>
       </c>
     </row>
+    <row r="113" spans="1:17">
+      <c r="A113" t="s">
+        <v>28</v>
+      </c>
+      <c r="B113" t="e">
+        <f>HLOOKUP(C113,D$107:G$109,D113)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C113">
+        <v>31</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="J113" s="1">
+        <v>2</v>
+      </c>
+      <c r="M113" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P113" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="Q113" t="b">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
     <row r="114" spans="1:17">
       <c r="A114" t="s">
-        <v>12</v>
-      </c>
-      <c r="B114" t="str">
-        <f>HLOOKUP(C114,D$114:G$116,1,FALSE)</f>
-        <v>one</v>
-      </c>
-      <c r="C114" t="s">
-        <v>12</v>
-      </c>
-      <c r="D114" t="s">
-        <v>12</v>
-      </c>
-      <c r="E114" t="s">
-        <v>13</v>
-      </c>
-      <c r="F114" t="s">
-        <v>32</v>
-      </c>
-      <c r="G114" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="B114" t="e">
+        <f>HLOOKUP(C114,D$107:G$109,D114)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C114">
+        <v>31</v>
+      </c>
+      <c r="D114">
+        <v>4</v>
       </c>
       <c r="J114" s="1">
-        <v>5</v>
-      </c>
-      <c r="K114" t="s">
-        <v>44</v>
-      </c>
-      <c r="L114" t="s">
-        <v>24</v>
+        <v>2</v>
+      </c>
+      <c r="M114" s="3" t="e">
+        <v>#REF!</v>
       </c>
       <c r="P114" t="b">
-        <f t="shared" ref="P114:P121" si="11">OR(ISBLANK(B114),IF(ISERROR(B114),ERROR.TYPE(B114)=IF(ISBLANK(M114),ERROR.TYPE(A114),ERROR.TYPE(M114)),IF(ISBLANK(M114),AND(NOT(ISBLANK(A114)),A114=B114),B114=M114)))</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="Q114" t="b">
-        <f t="shared" ref="Q114:Q122" si="12">IF(ISBLANK(O114),IF(ISERROR(P114),FALSE,P114),O114)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:17">
-      <c r="A115" t="s">
-        <v>35</v>
-      </c>
-      <c r="B115" t="str">
-        <f>HLOOKUP(C115,D$114:G$116,2,FALSE)</f>
-        <v>три</v>
-      </c>
-      <c r="C115" t="s">
-        <v>32</v>
-      </c>
-      <c r="D115" t="s">
-        <v>33</v>
-      </c>
-      <c r="E115" t="s">
-        <v>34</v>
-      </c>
-      <c r="F115" t="s">
-        <v>35</v>
-      </c>
-      <c r="G115" t="s">
-        <v>41</v>
-      </c>
-      <c r="J115" s="1">
-        <v>1</v>
-      </c>
-      <c r="P115" t="b">
-        <f t="shared" si="11"/>
-        <v>1</v>
-      </c>
-      <c r="Q115" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:17">
       <c r="A116" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B116" t="str">
-        <f>HLOOKUP(C116,D$114:G$116,3,FALSE)</f>
-        <v>vier</v>
+        <f>HLOOKUP(C116,D$116:G$118,1,FALSE)</f>
+        <v>one</v>
       </c>
       <c r="C116" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" t="s">
+        <v>13</v>
+      </c>
+      <c r="F116" t="s">
+        <v>32</v>
+      </c>
+      <c r="G116" t="s">
         <v>40</v>
       </c>
-      <c r="D116" t="s">
-        <v>36</v>
-      </c>
-      <c r="E116" t="s">
-        <v>37</v>
-      </c>
-      <c r="F116" t="s">
-        <v>38</v>
-      </c>
-      <c r="G116" t="s">
-        <v>42</v>
-      </c>
       <c r="J116" s="1">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="K116" t="s">
+        <v>44</v>
+      </c>
+      <c r="L116" t="s">
+        <v>24</v>
       </c>
       <c r="P116" t="b">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="P116:P123" si="11">OR(ISBLANK(B116),IF(ISERROR(B116),ERROR.TYPE(B116)=IF(ISBLANK(M116),ERROR.TYPE(A116),ERROR.TYPE(M116)),IF(ISBLANK(M116),AND(NOT(ISBLANK(A116)),A116=B116),B116=M116)))</f>
         <v>1</v>
       </c>
       <c r="Q116" t="b">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="Q116:Q124" si="12">IF(ISBLANK(O116),IF(ISERROR(P116),FALSE,P116),O116)</f>
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:17">
       <c r="A117" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="B117" t="str">
-        <f t="shared" ref="B117:B122" si="13">HLOOKUP(C117,D$114:G$116,D117,FALSE)</f>
-        <v>one</v>
+        <f>HLOOKUP(C117,D$116:G$118,2,FALSE)</f>
+        <v>три</v>
       </c>
       <c r="C117" t="s">
-        <v>12</v>
-      </c>
-      <c r="D117">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="D117" t="s">
+        <v>33</v>
+      </c>
+      <c r="E117" t="s">
+        <v>34</v>
+      </c>
+      <c r="F117" t="s">
+        <v>35</v>
+      </c>
+      <c r="G117" t="s">
+        <v>41</v>
       </c>
       <c r="J117" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P117" t="b">
         <f t="shared" si="11"/>
@@ -3668,261 +3712,264 @@
     </row>
     <row r="118" spans="1:17">
       <c r="A118" t="s">
+        <v>42</v>
+      </c>
+      <c r="B118" t="str">
+        <f>HLOOKUP(C118,D$116:G$118,3,FALSE)</f>
+        <v>vier</v>
+      </c>
+      <c r="C118" t="s">
+        <v>40</v>
+      </c>
+      <c r="D118" t="s">
+        <v>36</v>
+      </c>
+      <c r="E118" t="s">
+        <v>37</v>
+      </c>
+      <c r="F118" t="s">
+        <v>38</v>
+      </c>
+      <c r="G118" t="s">
+        <v>42</v>
+      </c>
+      <c r="J118" s="1">
+        <v>1</v>
+      </c>
+      <c r="P118" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q118" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
+      <c r="A119" t="s">
+        <v>12</v>
+      </c>
+      <c r="B119" t="str">
+        <f t="shared" ref="B119:B124" si="13">HLOOKUP(C119,D$116:G$118,D119,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C119" t="s">
+        <v>12</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="J119" s="1">
+        <v>2</v>
+      </c>
+      <c r="P119" t="b">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="Q119" t="b">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
+      <c r="A120" t="s">
         <v>35</v>
       </c>
-      <c r="B118" t="str">
+      <c r="B120" t="str">
         <f t="shared" si="13"/>
         <v>три</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C120" t="s">
         <v>32</v>
       </c>
-      <c r="D118">
-        <v>2</v>
-      </c>
-      <c r="J118" s="1">
-        <v>2</v>
-      </c>
-      <c r="P118" t="b">
+      <c r="D120">
+        <v>2</v>
+      </c>
+      <c r="J120" s="1">
+        <v>2</v>
+      </c>
+      <c r="P120" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q118" t="b">
+      <c r="Q120" t="b">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
-      <c r="A119" t="s">
+    <row r="121" spans="1:17">
+      <c r="A121" t="s">
         <v>42</v>
       </c>
-      <c r="B119" t="str">
+      <c r="B121" t="str">
         <f t="shared" si="13"/>
         <v>vier</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C121" t="s">
         <v>40</v>
       </c>
-      <c r="D119">
+      <c r="D121">
         <v>3</v>
       </c>
-      <c r="J119" s="1">
-        <v>2</v>
-      </c>
-      <c r="P119" t="b">
+      <c r="J121" s="1">
+        <v>2</v>
+      </c>
+      <c r="P121" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q119" t="b">
+      <c r="Q121" t="b">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
-      <c r="A120" t="s">
+    <row r="122" spans="1:17">
+      <c r="A122" t="s">
         <v>46</v>
       </c>
-      <c r="B120" t="e">
+      <c r="B122" t="e">
         <f t="shared" si="13"/>
         <v>#N/A</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C122" t="s">
         <v>43</v>
       </c>
-      <c r="D120">
-        <v>1</v>
-      </c>
-      <c r="J120" s="1">
-        <v>2</v>
-      </c>
-      <c r="M120" s="3" t="e">
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="J122" s="1">
+        <v>2</v>
+      </c>
+      <c r="M122" s="3" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P120" t="b">
-        <f>OR(ISBLANK(B120),IF(ISERROR(B120),ERROR.TYPE(B120)=IF(ISBLANK(M120),ERROR.TYPE(A120),ERROR.TYPE(M120)),IF(ISBLANK(M120),AND(NOT(ISBLANK(A120)),A120=B120),B120=M120)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q120" t="b">
+      <c r="P122" t="b">
+        <f>OR(ISBLANK(B122),IF(ISERROR(B122),ERROR.TYPE(B122)=IF(ISBLANK(M122),ERROR.TYPE(A122),ERROR.TYPE(M122)),IF(ISBLANK(M122),AND(NOT(ISBLANK(A122)),A122=B122),B122=M122)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q122" t="b">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
-      <c r="A121" t="s">
+    <row r="123" spans="1:17">
+      <c r="A123" t="s">
         <v>45</v>
       </c>
-      <c r="B121" t="e">
+      <c r="B123" t="e">
         <f t="shared" si="13"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C121" t="s">
-        <v>12</v>
-      </c>
-      <c r="D121">
+      <c r="C123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123">
         <v>0</v>
       </c>
-      <c r="J121" s="1">
-        <v>2</v>
-      </c>
-      <c r="M121" s="3" t="e">
+      <c r="J123" s="1">
+        <v>2</v>
+      </c>
+      <c r="M123" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P121" t="b">
+      <c r="P123" t="b">
         <f t="shared" si="11"/>
         <v>1</v>
       </c>
-      <c r="Q121" t="b">
+      <c r="Q123" t="b">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
-      <c r="A122" t="s">
+    <row r="124" spans="1:17">
+      <c r="A124" t="s">
         <v>45</v>
       </c>
-      <c r="B122" t="e">
+      <c r="B124" t="e">
         <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
-      <c r="C122" t="s">
-        <v>12</v>
-      </c>
-      <c r="D122">
-        <v>4</v>
-      </c>
-      <c r="J122" s="1">
-        <v>2</v>
-      </c>
-      <c r="M122" s="3" t="e">
+      <c r="C124" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124">
+        <v>4</v>
+      </c>
+      <c r="J124" s="1">
+        <v>2</v>
+      </c>
+      <c r="M124" s="3" t="e">
         <v>#REF!</v>
       </c>
-      <c r="P122" t="b">
-        <f>OR(ISBLANK(B122),IF(ISERROR(B122),ERROR.TYPE(B122)=IF(ISBLANK(M122),ERROR.TYPE(A122),ERROR.TYPE(M122)),IF(ISBLANK(M122),AND(NOT(ISBLANK(A122)),A122=B122),B122=M122)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q122" t="b">
+      <c r="P124" t="b">
+        <f>OR(ISBLANK(B124),IF(ISERROR(B124),ERROR.TYPE(B124)=IF(ISBLANK(M124),ERROR.TYPE(A124),ERROR.TYPE(M124)),IF(ISBLANK(M124),AND(NOT(ISBLANK(A124)),A124=B124),B124=M124)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q124" t="b">
         <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:17">
-      <c r="A124">
-        <v>22</v>
-      </c>
-      <c r="B124">
-        <f>VLOOKUP(C124,D$124:F$126,3)</f>
-        <v>22</v>
-      </c>
-      <c r="C124">
-        <v>29</v>
-      </c>
-      <c r="D124">
-        <v>10</v>
-      </c>
-      <c r="E124">
-        <v>11</v>
-      </c>
-      <c r="F124">
-        <v>21</v>
-      </c>
-      <c r="J124" s="1">
-        <v>4</v>
-      </c>
-      <c r="K124" t="s">
-        <v>25</v>
-      </c>
-      <c r="L124" t="s">
-        <v>25</v>
-      </c>
-      <c r="P124" t="b">
-        <f t="shared" ref="P124:P131" si="14">OR(ISBLANK(B124),IF(ISERROR(B124),ERROR.TYPE(B124)=IF(ISBLANK(M124),ERROR.TYPE(A124),ERROR.TYPE(M124)),IF(ISBLANK(M124),AND(NOT(ISBLANK(A124)),A124=B124),B124=M124)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q124" t="b">
-        <f t="shared" ref="Q124:Q131" si="15">IF(ISBLANK(O124),IF(ISERROR(P124),FALSE,P124),O124)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:17">
-      <c r="A125">
-        <v>23</v>
-      </c>
-      <c r="B125">
-        <f>VLOOKUP(C125,D$124:F$126,3)</f>
-        <v>23</v>
-      </c>
-      <c r="C125">
-        <v>30</v>
-      </c>
-      <c r="D125">
-        <v>20</v>
-      </c>
-      <c r="E125">
-        <v>12</v>
-      </c>
-      <c r="F125">
-        <v>22</v>
-      </c>
-      <c r="J125" s="1">
-        <v>1</v>
-      </c>
-      <c r="P125" t="b">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="Q125" t="b">
-        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:17">
       <c r="A126">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B126">
-        <f>VLOOKUP(C126,D$124:F$126,3)</f>
-        <v>23</v>
+        <f>VLOOKUP(C126,D$126:F$128,3)</f>
+        <v>22</v>
       </c>
       <c r="C126">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D126">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E126">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F126">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J126" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K126" t="s">
+        <v>25</v>
+      </c>
+      <c r="L126" t="s">
+        <v>25</v>
       </c>
       <c r="P126" t="b">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="P126:P133" si="14">OR(ISBLANK(B126),IF(ISERROR(B126),ERROR.TYPE(B126)=IF(ISBLANK(M126),ERROR.TYPE(A126),ERROR.TYPE(M126)),IF(ISBLANK(M126),AND(NOT(ISBLANK(A126)),A126=B126),B126=M126)))</f>
         <v>1</v>
       </c>
       <c r="Q126" t="b">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="Q126:Q133" si="15">IF(ISBLANK(O126),IF(ISERROR(P126),FALSE,P126),O126)</f>
         <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:17">
       <c r="A127">
+        <v>23</v>
+      </c>
+      <c r="B127">
+        <f>VLOOKUP(C127,D$126:F$128,3)</f>
+        <v>23</v>
+      </c>
+      <c r="C127">
+        <v>30</v>
+      </c>
+      <c r="D127">
         <v>20</v>
       </c>
-      <c r="B127">
-        <f>VLOOKUP(C127,D$124:F$126,D127)</f>
-        <v>20</v>
-      </c>
-      <c r="C127">
-        <v>29</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
+      <c r="E127">
+        <v>12</v>
+      </c>
+      <c r="F127">
+        <v>22</v>
       </c>
       <c r="J127" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P127" t="b">
         <f t="shared" si="14"/>
@@ -3935,20 +3982,26 @@
     </row>
     <row r="128" spans="1:17">
       <c r="A128">
+        <v>23</v>
+      </c>
+      <c r="B128">
+        <f>VLOOKUP(C128,D$126:F$128,3)</f>
+        <v>23</v>
+      </c>
+      <c r="C128">
+        <v>31</v>
+      </c>
+      <c r="D128">
+        <v>30</v>
+      </c>
+      <c r="E128">
         <v>13</v>
       </c>
-      <c r="B128">
-        <f>VLOOKUP(C128,D$124:F$126,D128)</f>
-        <v>13</v>
-      </c>
-      <c r="C128">
-        <v>30</v>
-      </c>
-      <c r="D128">
-        <v>2</v>
+      <c r="F128">
+        <v>23</v>
       </c>
       <c r="J128" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P128" t="b">
         <f t="shared" si="14"/>
@@ -3961,17 +4014,17 @@
     </row>
     <row r="129" spans="1:17">
       <c r="A129">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B129">
-        <f>VLOOKUP(C129,D$124:F$126,D129)</f>
-        <v>23</v>
+        <f>VLOOKUP(C129,D$126:F$128,D129)</f>
+        <v>20</v>
       </c>
       <c r="C129">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D129">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J129" s="1">
         <v>2</v>
@@ -3986,24 +4039,21 @@
       </c>
     </row>
     <row r="130" spans="1:17">
-      <c r="A130" t="s">
-        <v>28</v>
-      </c>
-      <c r="B130" t="e">
-        <f>VLOOKUP(C130,D$124:F$126,D130)</f>
-        <v>#VALUE!</v>
+      <c r="A130">
+        <v>13</v>
+      </c>
+      <c r="B130">
+        <f>VLOOKUP(C130,D$126:F$128,D130)</f>
+        <v>13</v>
       </c>
       <c r="C130">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J130" s="1">
         <v>2</v>
-      </c>
-      <c r="M130" s="3" t="e">
-        <v>#VALUE!</v>
       </c>
       <c r="P130" t="b">
         <f t="shared" si="14"/>
@@ -4015,24 +4065,21 @@
       </c>
     </row>
     <row r="131" spans="1:17">
-      <c r="A131" t="s">
-        <v>28</v>
-      </c>
-      <c r="B131" t="e">
-        <f>VLOOKUP(C131,D$124:F$126,D131)</f>
-        <v>#REF!</v>
+      <c r="A131">
+        <v>23</v>
+      </c>
+      <c r="B131">
+        <f>VLOOKUP(C131,D$126:F$128,D131)</f>
+        <v>23</v>
       </c>
       <c r="C131">
         <v>31</v>
       </c>
       <c r="D131">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J131" s="1">
         <v>2</v>
-      </c>
-      <c r="M131" s="3" t="e">
-        <v>#REF!</v>
       </c>
       <c r="P131" t="b">
         <f t="shared" si="14"/>
@@ -4044,126 +4091,126 @@
       </c>
     </row>
     <row r="132" spans="1:17">
-      <c r="M132" s="3"/>
+      <c r="A132" t="s">
+        <v>28</v>
+      </c>
+      <c r="B132" t="e">
+        <f>VLOOKUP(C132,D$126:F$128,D132)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C132">
+        <v>31</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="J132" s="1">
+        <v>2</v>
+      </c>
+      <c r="M132" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="P132" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="Q132" t="b">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="133" spans="1:17">
       <c r="A133" t="s">
-        <v>12</v>
-      </c>
-      <c r="B133" t="str">
-        <f>VLOOKUP(C133,D$133:F$135,1,FALSE)</f>
-        <v>one</v>
-      </c>
-      <c r="C133" t="s">
-        <v>12</v>
-      </c>
-      <c r="D133" t="s">
-        <v>12</v>
-      </c>
-      <c r="E133" t="s">
-        <v>33</v>
-      </c>
-      <c r="F133" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="B133" t="e">
+        <f>VLOOKUP(C133,D$126:F$128,D133)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C133">
+        <v>31</v>
+      </c>
+      <c r="D133">
+        <v>4</v>
       </c>
       <c r="J133" s="1">
-        <v>4</v>
-      </c>
-      <c r="K133" t="s">
-        <v>39</v>
-      </c>
-      <c r="L133" t="s">
-        <v>25</v>
+        <v>2</v>
+      </c>
+      <c r="M133" s="3" t="e">
+        <v>#REF!</v>
       </c>
       <c r="P133" t="b">
-        <f t="shared" ref="P133:P141" si="16">OR(ISBLANK(B133),IF(ISERROR(B133),ERROR.TYPE(B133)=IF(ISBLANK(M133),ERROR.TYPE(A133),ERROR.TYPE(M133)),IF(ISBLANK(M133),AND(NOT(ISBLANK(A133)),A133=B133),B133=M133)))</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="Q133" t="b">
-        <f t="shared" ref="Q133:Q141" si="17">IF(ISBLANK(O133),IF(ISERROR(P133),FALSE,P133),O133)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:17">
-      <c r="A134" t="s">
-        <v>34</v>
-      </c>
-      <c r="B134" t="str">
-        <f>VLOOKUP(C134,D$133:F$135,2,FALSE)</f>
-        <v>два</v>
-      </c>
-      <c r="C134" t="s">
-        <v>13</v>
-      </c>
-      <c r="D134" t="s">
-        <v>13</v>
-      </c>
-      <c r="E134" t="s">
-        <v>34</v>
-      </c>
-      <c r="F134" t="s">
-        <v>37</v>
-      </c>
-      <c r="J134" s="1">
-        <v>1</v>
-      </c>
-      <c r="P134" t="b">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
-      <c r="Q134" t="b">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
+      <c r="M134" s="3"/>
     </row>
     <row r="135" spans="1:17">
       <c r="A135" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B135" t="str">
-        <f>VLOOKUP(C135,D$133:F$135,3,FALSE)</f>
-        <v>drei</v>
+        <f>VLOOKUP(C135,D$135:F$137,1,FALSE)</f>
+        <v>one</v>
       </c>
       <c r="C135" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="D135" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="E135" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F135" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J135" s="1">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="K135" t="s">
+        <v>39</v>
+      </c>
+      <c r="L135" t="s">
+        <v>25</v>
       </c>
       <c r="P135" t="b">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="P135:P143" si="16">OR(ISBLANK(B135),IF(ISERROR(B135),ERROR.TYPE(B135)=IF(ISBLANK(M135),ERROR.TYPE(A135),ERROR.TYPE(M135)),IF(ISBLANK(M135),AND(NOT(ISBLANK(A135)),A135=B135),B135=M135)))</f>
         <v>1</v>
       </c>
       <c r="Q135" t="b">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="Q135:Q143" si="17">IF(ISBLANK(O135),IF(ISERROR(P135),FALSE,P135),O135)</f>
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:17">
       <c r="A136" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B136" t="str">
-        <f t="shared" ref="B136:B141" si="18">VLOOKUP(C136,D$133:F$135,D136,FALSE)</f>
-        <v>one</v>
+        <f>VLOOKUP(C136,D$135:F$137,2,FALSE)</f>
+        <v>два</v>
       </c>
       <c r="C136" t="s">
-        <v>12</v>
-      </c>
-      <c r="D136">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="D136" t="s">
+        <v>13</v>
+      </c>
+      <c r="E136" t="s">
+        <v>34</v>
+      </c>
+      <c r="F136" t="s">
+        <v>37</v>
       </c>
       <c r="J136" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P136" t="b">
         <f t="shared" si="16"/>
@@ -4176,454 +4223,509 @@
     </row>
     <row r="137" spans="1:17">
       <c r="A137" t="s">
+        <v>38</v>
+      </c>
+      <c r="B137" t="str">
+        <f>VLOOKUP(C137,D$135:F$137,3,FALSE)</f>
+        <v>drei</v>
+      </c>
+      <c r="C137" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137" t="s">
+        <v>32</v>
+      </c>
+      <c r="E137" t="s">
+        <v>35</v>
+      </c>
+      <c r="F137" t="s">
+        <v>38</v>
+      </c>
+      <c r="J137" s="1">
+        <v>1</v>
+      </c>
+      <c r="P137" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q137" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17">
+      <c r="A138" t="s">
+        <v>12</v>
+      </c>
+      <c r="B138" t="str">
+        <f t="shared" ref="B138:B143" si="18">VLOOKUP(C138,D$135:F$137,D138,FALSE)</f>
+        <v>one</v>
+      </c>
+      <c r="C138" t="s">
+        <v>12</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+      <c r="J138" s="1">
+        <v>2</v>
+      </c>
+      <c r="P138" t="b">
+        <f t="shared" si="16"/>
+        <v>1</v>
+      </c>
+      <c r="Q138" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:17">
+      <c r="A139" t="s">
         <v>34</v>
       </c>
-      <c r="B137" t="str">
+      <c r="B139" t="str">
         <f t="shared" si="18"/>
         <v>два</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C139" t="s">
         <v>13</v>
       </c>
-      <c r="D137">
-        <v>2</v>
-      </c>
-      <c r="J137" s="1">
-        <v>2</v>
-      </c>
-      <c r="P137" t="b">
+      <c r="D139">
+        <v>2</v>
+      </c>
+      <c r="J139" s="1">
+        <v>2</v>
+      </c>
+      <c r="P139" t="b">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q137" t="b">
+      <c r="Q139" t="b">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
-      <c r="A138" t="s">
+    <row r="140" spans="1:17">
+      <c r="A140" t="s">
         <v>38</v>
       </c>
-      <c r="B138" t="str">
+      <c r="B140" t="str">
         <f t="shared" si="18"/>
         <v>drei</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C140" t="s">
         <v>32</v>
       </c>
-      <c r="D138">
+      <c r="D140">
         <v>3</v>
       </c>
-      <c r="J138" s="1">
-        <v>2</v>
-      </c>
-      <c r="P138" t="b">
+      <c r="J140" s="1">
+        <v>2</v>
+      </c>
+      <c r="P140" t="b">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q138" t="b">
+      <c r="Q140" t="b">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
-      <c r="A139" t="s">
+    <row r="141" spans="1:17">
+      <c r="A141" t="s">
         <v>46</v>
       </c>
-      <c r="B139" t="e">
+      <c r="B141" t="e">
         <f t="shared" si="18"/>
         <v>#N/A</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C141" t="s">
         <v>40</v>
       </c>
-      <c r="D139">
-        <v>1</v>
-      </c>
-      <c r="J139" s="1">
-        <v>2</v>
-      </c>
-      <c r="M139" s="3" t="e">
+      <c r="D141">
+        <v>1</v>
+      </c>
+      <c r="J141" s="1">
+        <v>2</v>
+      </c>
+      <c r="M141" s="3" t="e">
         <v>#N/A</v>
       </c>
-      <c r="P139" t="b">
+      <c r="P141" t="b">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q139" t="b">
+      <c r="Q141" t="b">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
-      <c r="A140" t="s">
+    <row r="142" spans="1:17">
+      <c r="A142" t="s">
         <v>45</v>
       </c>
-      <c r="B140" t="e">
+      <c r="B142" t="e">
         <f t="shared" si="18"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C140" t="s">
-        <v>12</v>
-      </c>
-      <c r="D140">
+      <c r="C142" t="s">
+        <v>12</v>
+      </c>
+      <c r="D142">
         <v>0</v>
       </c>
-      <c r="J140" s="1">
-        <v>2</v>
-      </c>
-      <c r="M140" s="3" t="e">
+      <c r="J142" s="1">
+        <v>2</v>
+      </c>
+      <c r="M142" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P140" t="b">
+      <c r="P142" t="b">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q140" t="b">
+      <c r="Q142" t="b">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
-      <c r="A141" t="s">
+    <row r="143" spans="1:17">
+      <c r="A143" t="s">
         <v>45</v>
       </c>
-      <c r="B141" t="e">
+      <c r="B143" t="e">
         <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
-      <c r="C141" t="s">
-        <v>12</v>
-      </c>
-      <c r="D141">
-        <v>4</v>
-      </c>
-      <c r="J141" s="1">
-        <v>2</v>
-      </c>
-      <c r="M141" s="3" t="e">
+      <c r="C143" t="s">
+        <v>12</v>
+      </c>
+      <c r="D143">
+        <v>4</v>
+      </c>
+      <c r="J143" s="1">
+        <v>2</v>
+      </c>
+      <c r="M143" s="3" t="e">
         <v>#REF!</v>
       </c>
-      <c r="P141" t="b">
+      <c r="P143" t="b">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q141" t="b">
+      <c r="Q143" t="b">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
-      <c r="M142" s="3"/>
-    </row>
-    <row r="143" spans="1:17">
-      <c r="A143">
+    <row r="144" spans="1:17">
+      <c r="M144" s="3"/>
+    </row>
+    <row r="145" spans="1:17">
+      <c r="A145">
         <v>11</v>
       </c>
-      <c r="B143">
-        <f t="shared" ref="B143:B148" si="19">CHOOSE(C143,D143,E143,F143)</f>
+      <c r="B145">
+        <f t="shared" ref="B145:B150" si="19">CHOOSE(C145,D145,E145,F145)</f>
         <v>11</v>
       </c>
-      <c r="C143">
-        <v>1</v>
-      </c>
-      <c r="D143">
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145">
         <v>11</v>
       </c>
-      <c r="E143">
-        <v>12</v>
-      </c>
-      <c r="F143">
+      <c r="E145">
+        <v>12</v>
+      </c>
+      <c r="F145">
         <v>13</v>
       </c>
-      <c r="J143" s="1">
-        <v>4</v>
-      </c>
-      <c r="K143" t="s">
+      <c r="J145" s="1">
+        <v>4</v>
+      </c>
+      <c r="K145" t="s">
         <v>26</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L145" t="s">
         <v>26</v>
       </c>
-      <c r="M143" s="3"/>
-      <c r="P143" t="b">
-        <f t="shared" ref="P143:P148" si="20">OR(ISBLANK(B143),IF(ISERROR(B143),ERROR.TYPE(B143)=IF(ISBLANK(M143),ERROR.TYPE(A143),ERROR.TYPE(M143)),IF(ISBLANK(M143),AND(NOT(ISBLANK(A143)),A143=B143),B143=M143)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q143" t="b">
-        <f t="shared" ref="Q143:Q148" si="21">IF(ISBLANK(O143),IF(ISERROR(P143),FALSE,P143),O143)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:17">
-      <c r="A144">
+      <c r="M145" s="3"/>
+      <c r="P145" t="b">
+        <f t="shared" ref="P145:P150" si="20">OR(ISBLANK(B145),IF(ISERROR(B145),ERROR.TYPE(B145)=IF(ISBLANK(M145),ERROR.TYPE(A145),ERROR.TYPE(M145)),IF(ISBLANK(M145),AND(NOT(ISBLANK(A145)),A145=B145),B145=M145)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q145" t="b">
+        <f t="shared" ref="Q145:Q150" si="21">IF(ISBLANK(O145),IF(ISERROR(P145),FALSE,P145),O145)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:17">
+      <c r="A146">
         <v>22</v>
       </c>
-      <c r="B144">
+      <c r="B146">
         <f t="shared" si="19"/>
         <v>22</v>
       </c>
-      <c r="C144">
-        <v>2</v>
-      </c>
-      <c r="D144">
+      <c r="C146">
+        <v>2</v>
+      </c>
+      <c r="D146">
         <v>21</v>
       </c>
-      <c r="E144">
+      <c r="E146">
         <v>22</v>
       </c>
-      <c r="F144">
+      <c r="F146">
         <v>23</v>
       </c>
-      <c r="J144" s="1">
-        <v>4</v>
-      </c>
-      <c r="P144" t="b">
+      <c r="J146" s="1">
+        <v>4</v>
+      </c>
+      <c r="P146" t="b">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="Q144" t="b">
+      <c r="Q146" t="b">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
-      <c r="A145">
+    <row r="147" spans="1:17">
+      <c r="A147">
         <v>33</v>
       </c>
-      <c r="B145">
+      <c r="B147">
         <f t="shared" si="19"/>
         <v>33</v>
       </c>
-      <c r="C145">
+      <c r="C147">
         <v>3</v>
       </c>
-      <c r="D145">
+      <c r="D147">
         <v>31</v>
       </c>
-      <c r="E145">
+      <c r="E147">
         <v>32</v>
       </c>
-      <c r="F145">
+      <c r="F147">
         <v>33</v>
       </c>
-      <c r="J145" s="1">
-        <v>4</v>
-      </c>
-      <c r="P145" t="b">
+      <c r="J147" s="1">
+        <v>4</v>
+      </c>
+      <c r="P147" t="b">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="Q145" t="b">
+      <c r="Q147" t="b">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
-      <c r="A146" t="s">
+    <row r="148" spans="1:17">
+      <c r="A148" t="s">
         <v>28</v>
       </c>
-      <c r="B146" t="e">
+      <c r="B148" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C146">
-        <v>4</v>
-      </c>
-      <c r="D146">
+      <c r="C148">
+        <v>4</v>
+      </c>
+      <c r="D148">
         <v>11</v>
       </c>
-      <c r="E146">
-        <v>12</v>
-      </c>
-      <c r="F146">
+      <c r="E148">
+        <v>12</v>
+      </c>
+      <c r="F148">
         <v>13</v>
       </c>
-      <c r="J146" s="1">
-        <v>4</v>
-      </c>
-      <c r="M146" s="3" t="e">
+      <c r="J148" s="1">
+        <v>4</v>
+      </c>
+      <c r="M148" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P146" t="b">
+      <c r="P148" t="b">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="Q146" t="b">
+      <c r="Q148" t="b">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
-      <c r="A147" t="s">
+    <row r="149" spans="1:17">
+      <c r="A149" t="s">
         <v>28</v>
       </c>
-      <c r="B147" t="e">
+      <c r="B149" t="e">
         <f t="shared" si="19"/>
         <v>#VALUE!</v>
       </c>
-      <c r="C147">
+      <c r="C149">
         <v>0</v>
       </c>
-      <c r="D147">
+      <c r="D149">
         <v>11</v>
       </c>
-      <c r="E147">
-        <v>12</v>
-      </c>
-      <c r="F147">
+      <c r="E149">
+        <v>12</v>
+      </c>
+      <c r="F149">
         <v>13</v>
       </c>
-      <c r="J147" s="1">
-        <v>4</v>
-      </c>
-      <c r="M147" s="3" t="e">
+      <c r="J149" s="1">
+        <v>4</v>
+      </c>
+      <c r="M149" s="3" t="e">
         <v>#VALUE!</v>
       </c>
-      <c r="P147" t="b">
+      <c r="P149" t="b">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="Q147" t="b">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17">
-      <c r="A148">
-        <v>12</v>
-      </c>
-      <c r="B148">
-        <f t="shared" si="19"/>
-        <v>12</v>
-      </c>
-      <c r="C148">
-        <v>2.99</v>
-      </c>
-      <c r="D148">
-        <v>11</v>
-      </c>
-      <c r="E148">
-        <v>12</v>
-      </c>
-      <c r="F148">
-        <v>13</v>
-      </c>
-      <c r="J148" s="1">
-        <v>4</v>
-      </c>
-      <c r="P148" t="b">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-      <c r="Q148" t="b">
+      <c r="Q149" t="b">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:17">
       <c r="A150">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B150">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="C150">
+        <v>2.99</v>
+      </c>
+      <c r="D150">
+        <v>11</v>
+      </c>
+      <c r="E150">
+        <v>12</v>
+      </c>
+      <c r="F150">
+        <v>13</v>
+      </c>
+      <c r="J150" s="1">
+        <v>4</v>
+      </c>
+      <c r="P150" t="b">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="Q150" t="b">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:17">
+      <c r="A152">
+        <v>2</v>
+      </c>
+      <c r="B152">
         <f>COLUMN()</f>
         <v>2</v>
       </c>
-      <c r="J150" s="1">
+      <c r="J152" s="1">
         <v>0</v>
       </c>
-      <c r="K150" t="s">
+      <c r="K152" t="s">
         <v>47</v>
       </c>
-      <c r="L150" t="s">
+      <c r="L152" t="s">
         <v>47</v>
       </c>
-      <c r="P150" t="b">
-        <f t="shared" ref="P150:P151" si="22">OR(ISBLANK(B150),IF(ISERROR(B150),ERROR.TYPE(B150)=IF(ISBLANK(M150),ERROR.TYPE(A150),ERROR.TYPE(M150)),IF(ISBLANK(M150),AND(NOT(ISBLANK(A150)),A150=B150),B150=M150)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q150" t="b">
-        <f t="shared" ref="Q150:Q151" si="23">IF(ISBLANK(O150),IF(ISERROR(P150),FALSE,P150),O150)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:17">
-      <c r="A151">
-        <v>3</v>
-      </c>
-      <c r="B151">
-        <f>COLUMN(C151)</f>
-        <v>3</v>
-      </c>
-      <c r="J151" s="1">
-        <v>1</v>
-      </c>
-      <c r="P151" t="b">
-        <f t="shared" si="22"/>
-        <v>1</v>
-      </c>
-      <c r="Q151" t="b">
-        <f t="shared" si="23"/>
+      <c r="P152" t="b">
+        <f t="shared" ref="P152:P153" si="22">OR(ISBLANK(B152),IF(ISERROR(B152),ERROR.TYPE(B152)=IF(ISBLANK(M152),ERROR.TYPE(A152),ERROR.TYPE(M152)),IF(ISBLANK(M152),AND(NOT(ISBLANK(A152)),A152=B152),B152=M152)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q152" t="b">
+        <f t="shared" ref="Q152:Q153" si="23">IF(ISBLANK(O152),IF(ISERROR(P152),FALSE,P152),O152)</f>
         <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:17">
       <c r="A153">
-        <v>153</v>
+        <v>3</v>
       </c>
       <c r="B153">
+        <f>COLUMN(C153)</f>
+        <v>3</v>
+      </c>
+      <c r="J153" s="1">
+        <v>1</v>
+      </c>
+      <c r="P153" t="b">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="Q153" t="b">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17">
+      <c r="A155">
+        <v>155</v>
+      </c>
+      <c r="B155">
         <f>ROW()</f>
-        <v>153</v>
-      </c>
-      <c r="J153" s="1">
+        <v>155</v>
+      </c>
+      <c r="J155" s="1">
         <v>0</v>
       </c>
-      <c r="K153" t="s">
+      <c r="K155" t="s">
         <v>48</v>
       </c>
-      <c r="L153" t="s">
+      <c r="L155" t="s">
         <v>48</v>
       </c>
-      <c r="P153" t="b">
-        <f t="shared" ref="P153:P154" si="24">OR(ISBLANK(B153),IF(ISERROR(B153),ERROR.TYPE(B153)=IF(ISBLANK(M153),ERROR.TYPE(A153),ERROR.TYPE(M153)),IF(ISBLANK(M153),AND(NOT(ISBLANK(A153)),A153=B153),B153=M153)))</f>
-        <v>1</v>
-      </c>
-      <c r="Q153" t="b">
-        <f t="shared" ref="Q153:Q154" si="25">IF(ISBLANK(O153),IF(ISERROR(P153),FALSE,P153),O153)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17">
-      <c r="A154">
-        <v>154</v>
-      </c>
-      <c r="B154">
-        <f>ROW(C154)</f>
-        <v>154</v>
-      </c>
-      <c r="J154" s="1">
-        <v>1</v>
-      </c>
-      <c r="P154" t="b">
+      <c r="P155" t="b">
+        <f t="shared" ref="P155:P156" si="24">OR(ISBLANK(B155),IF(ISERROR(B155),ERROR.TYPE(B155)=IF(ISBLANK(M155),ERROR.TYPE(A155),ERROR.TYPE(M155)),IF(ISBLANK(M155),AND(NOT(ISBLANK(A155)),A155=B155),B155=M155)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q155" t="b">
+        <f t="shared" ref="Q155:Q156" si="25">IF(ISBLANK(O155),IF(ISERROR(P155),FALSE,P155),O155)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17">
+      <c r="A156">
+        <v>156</v>
+      </c>
+      <c r="B156">
+        <f>ROW(C156)</f>
+        <v>156</v>
+      </c>
+      <c r="J156" s="1">
+        <v>1</v>
+      </c>
+      <c r="P156" t="b">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="Q154" t="b">
+      <c r="Q156" t="b">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="13:13">
-      <c r="M162" s="3"/>
-    </row>
-    <row r="166" spans="13:13">
-      <c r="M166" s="3"/>
+    <row r="164" spans="13:13">
+      <c r="M164" s="3"/>
     </row>
     <row r="168" spans="13:13">
       <c r="M168" s="3"/>
     </row>
-    <row r="169" spans="13:13">
-      <c r="M169" s="3"/>
+    <row r="170" spans="13:13">
+      <c r="M170" s="3"/>
     </row>
     <row r="171" spans="13:13">
       <c r="M171" s="3"/>
@@ -4631,14 +4733,11 @@
     <row r="173" spans="13:13">
       <c r="M173" s="3"/>
     </row>
-    <row r="174" spans="13:13">
-      <c r="M174" s="3"/>
-    </row>
-    <row r="178" spans="13:13">
-      <c r="M178" s="3"/>
-    </row>
-    <row r="179" spans="13:13">
-      <c r="M179" s="3"/>
+    <row r="175" spans="13:13">
+      <c r="M175" s="3"/>
+    </row>
+    <row r="176" spans="13:13">
+      <c r="M176" s="3"/>
     </row>
     <row r="180" spans="13:13">
       <c r="M180" s="3"/>
@@ -4700,24 +4799,48 @@
     <row r="199" spans="13:13">
       <c r="M199" s="3"/>
     </row>
+    <row r="200" spans="13:13">
+      <c r="M200" s="3"/>
+    </row>
+    <row r="201" spans="13:13">
+      <c r="M201" s="3"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A2:A10029">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A2:A10031">
+    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I10029">
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+  <conditionalFormatting sqref="C2:I10031">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M10029">
-    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="M2:M10031">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A82:A83">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q82),Q82))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M82),ISBLANK(O82)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83 I82:I83 C82:G83">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>$J82&gt;COLUMN(C82)-3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M82:M83">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M82)),IF(ISERROR(A82),ERROR.TYPE(A82)=ERROR.TYPE(M82),A82=M82))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
compiler: Implement ADDRESS function.
</commit_message>
<xml_diff>
--- a/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
+++ b/components/system/src/test-reference/data/org/formulacompiler/tests/reference/LookupFunctions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="69">
   <si>
     <t>Actual</t>
   </si>
@@ -170,6 +170,57 @@
   </si>
   <si>
     <t>MATCH (descending, trailing NULLs)</t>
+  </si>
+  <si>
+    <t>Sheet1!$C$2</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>Sheet1!R2C3</t>
+  </si>
+  <si>
+    <t>'Sheet 2'!$C$2</t>
+  </si>
+  <si>
+    <t>Sheet 2</t>
+  </si>
+  <si>
+    <t>'Sheet''3'!R2C3</t>
+  </si>
+  <si>
+    <t>Sheet'3</t>
+  </si>
+  <si>
+    <t>C$2</t>
+  </si>
+  <si>
+    <t>$C2</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>R2C[3]</t>
+  </si>
+  <si>
+    <t>R[2]C3</t>
+  </si>
+  <si>
+    <t>R[2]C[3]</t>
+  </si>
+  <si>
+    <t>R[-2]C[-1]</t>
+  </si>
+  <si>
+    <t>IV55555</t>
+  </si>
+  <si>
+    <t>$DX$56</t>
   </si>
 </sst>
 </file>
@@ -235,7 +286,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="34"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="27"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="29"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -640,9 +747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q205"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -4897,16 +5002,440 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="13:13">
-      <c r="M168" s="3"/>
-    </row>
-    <row r="172" spans="13:13">
-      <c r="M172" s="3"/>
-    </row>
-    <row r="174" spans="13:13">
+    <row r="162" spans="1:17">
+      <c r="A162" t="s">
+        <v>52</v>
+      </c>
+      <c r="B162" t="str">
+        <f>ADDRESS(C162,D162,E162,F162,G162)</f>
+        <v>Sheet1!$C$2</v>
+      </c>
+      <c r="C162">
+        <v>2</v>
+      </c>
+      <c r="D162">
+        <v>3</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162" t="b">
+        <v>1</v>
+      </c>
+      <c r="G162" t="s">
+        <v>53</v>
+      </c>
+      <c r="J162" s="1">
+        <v>5</v>
+      </c>
+      <c r="K162" t="s">
+        <v>54</v>
+      </c>
+      <c r="L162" t="s">
+        <v>54</v>
+      </c>
+      <c r="P162" t="b">
+        <f t="shared" ref="P162:P172" si="26">OR(ISBLANK(B162),IF(ISERROR(B162),ERROR.TYPE(B162)=IF(ISBLANK(M162),ERROR.TYPE(A162),ERROR.TYPE(M162)),IF(ISBLANK(M162),AND(NOT(ISBLANK(A162)),A162=B162),B162=M162)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q162" t="b">
+        <f t="shared" ref="Q162:Q174" si="27">IF(ISBLANK(O162),IF(ISERROR(P162),FALSE,P162),O162)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17">
+      <c r="A163" t="s">
+        <v>55</v>
+      </c>
+      <c r="B163" t="str">
+        <f>ADDRESS(C163,D163,E163,F163,G163)</f>
+        <v>Sheet1!R2C3</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>3</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163" t="b">
+        <v>0</v>
+      </c>
+      <c r="G163" t="s">
+        <v>53</v>
+      </c>
+      <c r="J163" s="1">
+        <v>5</v>
+      </c>
+      <c r="P163" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q163" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:17">
+      <c r="A164" t="s">
+        <v>56</v>
+      </c>
+      <c r="B164" t="str">
+        <f>ADDRESS(C164,D164,E164,F164,G164)</f>
+        <v>'Sheet 2'!$C$2</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>3</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164" t="b">
+        <v>1</v>
+      </c>
+      <c r="G164" t="s">
+        <v>57</v>
+      </c>
+      <c r="J164" s="1">
+        <v>5</v>
+      </c>
+      <c r="K164" t="s">
+        <v>54</v>
+      </c>
+      <c r="L164" t="s">
+        <v>54</v>
+      </c>
+      <c r="P164" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q164" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17">
+      <c r="A165" t="s">
+        <v>58</v>
+      </c>
+      <c r="B165" t="str">
+        <f>ADDRESS(C165,D165,E165,F165,G165)</f>
+        <v>'Sheet''3'!R2C3</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+      <c r="D165">
+        <v>3</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165" t="b">
+        <v>0</v>
+      </c>
+      <c r="G165" t="s">
+        <v>59</v>
+      </c>
+      <c r="J165" s="1">
+        <v>5</v>
+      </c>
+      <c r="P165" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q165" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17">
+      <c r="A166" t="s">
+        <v>60</v>
+      </c>
+      <c r="B166" t="str">
+        <f t="shared" ref="B166:B172" si="28">ADDRESS(C166,D166,E166,F166)</f>
+        <v>C$2</v>
+      </c>
+      <c r="C166">
+        <v>2</v>
+      </c>
+      <c r="D166">
+        <v>3</v>
+      </c>
+      <c r="E166">
+        <v>2</v>
+      </c>
+      <c r="F166" t="b">
+        <v>1</v>
+      </c>
+      <c r="J166" s="1">
+        <v>4</v>
+      </c>
+      <c r="P166" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q166" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17">
+      <c r="A167" t="s">
+        <v>61</v>
+      </c>
+      <c r="B167" t="str">
+        <f t="shared" si="28"/>
+        <v>$C2</v>
+      </c>
+      <c r="C167">
+        <v>2</v>
+      </c>
+      <c r="D167">
+        <v>3</v>
+      </c>
+      <c r="E167">
+        <v>3</v>
+      </c>
+      <c r="F167" t="b">
+        <v>1</v>
+      </c>
+      <c r="J167" s="1">
+        <v>4</v>
+      </c>
+      <c r="P167" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q167" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17">
+      <c r="A168" t="s">
+        <v>62</v>
+      </c>
+      <c r="B168" t="str">
+        <f t="shared" si="28"/>
+        <v>C2</v>
+      </c>
+      <c r="C168">
+        <v>2</v>
+      </c>
+      <c r="D168">
+        <v>3</v>
+      </c>
+      <c r="E168">
+        <v>4</v>
+      </c>
+      <c r="F168" t="b">
+        <v>1</v>
+      </c>
+      <c r="J168" s="1">
+        <v>4</v>
+      </c>
+      <c r="P168" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q168" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17">
+      <c r="A169" t="s">
+        <v>63</v>
+      </c>
+      <c r="B169" t="str">
+        <f t="shared" si="28"/>
+        <v>R2C[3]</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+      <c r="D169">
+        <v>3</v>
+      </c>
+      <c r="E169">
+        <v>2</v>
+      </c>
+      <c r="F169" t="b">
+        <v>0</v>
+      </c>
+      <c r="J169" s="1">
+        <v>4</v>
+      </c>
+      <c r="P169" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q169" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:17">
+      <c r="A170" t="s">
+        <v>64</v>
+      </c>
+      <c r="B170" t="str">
+        <f t="shared" si="28"/>
+        <v>R[2]C3</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
+      </c>
+      <c r="D170">
+        <v>3</v>
+      </c>
+      <c r="E170">
+        <v>3</v>
+      </c>
+      <c r="F170" t="b">
+        <v>0</v>
+      </c>
+      <c r="J170" s="1">
+        <v>4</v>
+      </c>
+      <c r="M170" s="3"/>
+      <c r="P170" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q170" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:17">
+      <c r="A171" t="s">
+        <v>65</v>
+      </c>
+      <c r="B171" t="str">
+        <f t="shared" si="28"/>
+        <v>R[2]C[3]</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>3</v>
+      </c>
+      <c r="E171">
+        <v>4</v>
+      </c>
+      <c r="F171" t="b">
+        <v>0</v>
+      </c>
+      <c r="J171" s="1">
+        <v>4</v>
+      </c>
+      <c r="P171" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q171" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17">
+      <c r="A172" t="s">
+        <v>66</v>
+      </c>
+      <c r="B172" t="str">
+        <f t="shared" si="28"/>
+        <v>R[-2]C[-1]</v>
+      </c>
+      <c r="C172">
+        <v>-2</v>
+      </c>
+      <c r="D172">
+        <v>-1</v>
+      </c>
+      <c r="E172">
+        <v>4</v>
+      </c>
+      <c r="F172" t="b">
+        <v>0</v>
+      </c>
+      <c r="J172" s="1">
+        <v>4</v>
+      </c>
+      <c r="P172" t="b">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="Q172" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:17">
+      <c r="A173" t="s">
+        <v>67</v>
+      </c>
+      <c r="B173" t="str">
+        <f>ADDRESS(C173,D173,E173)</f>
+        <v>IV55555</v>
+      </c>
+      <c r="C173">
+        <v>55555</v>
+      </c>
+      <c r="D173">
+        <v>256</v>
+      </c>
+      <c r="E173">
+        <v>4</v>
+      </c>
+      <c r="J173" s="1">
+        <v>3</v>
+      </c>
+      <c r="P173" t="b">
+        <f>OR(ISBLANK(B173),IF(ISERROR(B173),ERROR.TYPE(B173)=IF(ISBLANK(M173),ERROR.TYPE(A173),ERROR.TYPE(M173)),IF(ISBLANK(M173),AND(NOT(ISBLANK(A173)),A173=B173),B173=M173)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q173" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17">
+      <c r="A174" t="s">
+        <v>68</v>
+      </c>
+      <c r="B174" t="str">
+        <f>ADDRESS(C174,D174)</f>
+        <v>$DX$56</v>
+      </c>
+      <c r="C174">
+        <v>56</v>
+      </c>
+      <c r="D174">
+        <v>128</v>
+      </c>
+      <c r="J174" s="1">
+        <v>2</v>
+      </c>
       <c r="M174" s="3"/>
-    </row>
-    <row r="175" spans="13:13">
+      <c r="P174" t="b">
+        <f>OR(ISBLANK(B174),IF(ISERROR(B174),ERROR.TYPE(B174)=IF(ISBLANK(M174),ERROR.TYPE(A174),ERROR.TYPE(M174)),IF(ISBLANK(M174),AND(NOT(ISBLANK(A174)),A174=B174),B174=M174)))</f>
+        <v>1</v>
+      </c>
+      <c r="Q174" t="b">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17">
       <c r="M175" s="3"/>
     </row>
     <row r="177" spans="13:13">
@@ -4987,75 +5516,93 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A2:A10035">
-    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="17" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q2),Q2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="18" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M2),ISBLANK(O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:I10035">
-    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
       <formula>$J2&gt;COLUMN(C2)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M10035">
-    <cfRule type="expression" dxfId="12" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="20" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M2)),IF(ISERROR(A2),ERROR.TYPE(A2)=ERROR.TYPE(M2),A2=M2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A86:A87">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="15" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q86),Q86))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="16" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M86),ISBLANK(O86)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H87 I86:I87 C86:G87">
-    <cfRule type="expression" dxfId="9" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="14" stopIfTrue="1">
       <formula>$J86&gt;COLUMN(C86)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M86:M87">
-    <cfRule type="expression" dxfId="8" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="13" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M86)),IF(ISERROR(A86),ERROR.TYPE(A86)=ERROR.TYPE(M86),A86=M86))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="11" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q12),Q12))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="12" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M12),ISBLANK(O12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:I13">
-    <cfRule type="expression" dxfId="5" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
       <formula>$J12&gt;COLUMN(C12)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12:M13">
-    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="9" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M12)),IF(ISERROR(A12),ERROR.TYPE(A12)=ERROR.TYPE(M12),A12=M12))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:A26">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>NOT(OR(ISBLANK(Q25),Q25))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>NOT(AND(ISBLANK(M25),ISBLANK(O25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:I26">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
       <formula>$J25&gt;COLUMN(C25)-3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M25:M26">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="5" stopIfTrue="1">
       <formula>AND(NOT(ISBLANK(M25)),IF(ISERROR(A25),ERROR.TYPE(A25)=ERROR.TYPE(M25),A25=M25))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A162:A174">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>NOT(OR(ISBLANK(Q162),Q162))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+      <formula>NOT(AND(ISBLANK(M162),ISBLANK(O162)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C162:I174">
+    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+      <formula>$J162&gt;COLUMN(C162)-3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M162:M174">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>AND(NOT(ISBLANK(M162)),IF(ISERROR(A162),ERROR.TYPE(A162)=ERROR.TYPE(M162),A162=M162))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>